<commit_message>
Do measurement code should be there.
</commit_message>
<xml_diff>
--- a/data_health_insurance.xlsx
+++ b/data_health_insurance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marij\PycharmProjects\health_insurance_cloud_networking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508EDB59-18AA-46E2-B89D-4A30ED6C34B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9583B5-6C1B-461D-B106-BDDED764EA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,9 +446,6 @@
     <t>Ideas for graph</t>
   </si>
   <si>
-    <t>https://scheepvaartnet.nl/azvz-zorgverzekering/aanvraagformulier-azvz/</t>
-  </si>
-  <si>
     <t>Home cookies</t>
   </si>
   <si>
@@ -1178,9 +1175,6 @@
     <t>Registration IPv4</t>
   </si>
   <si>
-    <t>https://service.zorgenzekerheid.nl/advies/uwnawgegevens.html</t>
-  </si>
-  <si>
     <t>193.173.52.131</t>
   </si>
   <si>
@@ -1416,6 +1410,12 @@
   </si>
   <si>
     <t>www.service.zorgenzekerheid.nl</t>
+  </si>
+  <si>
+    <t>https://www.scheepvaartnet.nl/azvz-zorgverzekering/aanvraagformulier-azvz/</t>
+  </si>
+  <si>
+    <t>https://www.service.zorgenzekerheid.nl/advies/uwnawgegevens.html</t>
   </si>
 </sst>
 </file>
@@ -1558,6 +1558,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <fgColor theme="7" tint="0.79998168889431442"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
@@ -1637,6 +1644,7 @@
     <dxf>
       <fill>
         <patternFill>
+          <fgColor theme="7" tint="0.79998168889431442"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1644,7 +1652,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1688,7 +1695,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1696,13 +1702,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
+          <fgColor theme="7" tint="0.79998168889431442"/>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -2132,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF24" sqref="AF24"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AZ6" sqref="AZ6:AZ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,211 +2215,211 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" t="s">
         <v>149</v>
-      </c>
-      <c r="G1" t="s">
-        <v>150</v>
       </c>
       <c r="H1" t="s">
         <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" t="s">
+        <v>350</v>
+      </c>
+      <c r="M1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s">
         <v>170</v>
       </c>
-      <c r="L1" t="s">
-        <v>351</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T1" t="s">
+        <v>172</v>
+      </c>
+      <c r="U1" t="s">
+        <v>173</v>
+      </c>
+      <c r="V1" t="s">
+        <v>174</v>
+      </c>
+      <c r="W1" t="s">
         <v>184</v>
       </c>
-      <c r="N1" t="s">
-        <v>177</v>
-      </c>
-      <c r="O1" t="s">
-        <v>199</v>
-      </c>
-      <c r="P1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>170</v>
-      </c>
-      <c r="R1" t="s">
-        <v>171</v>
-      </c>
-      <c r="S1" t="s">
-        <v>172</v>
-      </c>
-      <c r="T1" t="s">
-        <v>173</v>
-      </c>
-      <c r="U1" t="s">
-        <v>174</v>
-      </c>
-      <c r="V1" t="s">
-        <v>175</v>
-      </c>
-      <c r="W1" t="s">
-        <v>185</v>
-      </c>
       <c r="X1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Z1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA1" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>137</v>
       </c>
-      <c r="AB1" t="s">
-        <v>138</v>
-      </c>
       <c r="AC1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AD1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AE1" t="s">
         <v>133</v>
       </c>
       <c r="AF1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="AG1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AH1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO1" t="s">
         <v>162</v>
       </c>
-      <c r="AI1" t="s">
-        <v>381</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>376</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>409</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>447</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>266</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>267</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>287</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>288</v>
+      </c>
+      <c r="BG1" t="s">
         <v>201</v>
       </c>
-      <c r="AN1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>166</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>377</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>411</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>449</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>267</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>268</v>
-      </c>
-      <c r="BD1" t="s">
+      <c r="BH1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BP1" t="s">
         <v>143</v>
       </c>
-      <c r="BE1" t="s">
-        <v>288</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>289</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>202</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>203</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>151</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>152</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>153</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>154</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>155</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
+        <v>342</v>
+      </c>
+      <c r="BR1" t="s">
         <v>157</v>
       </c>
-      <c r="BP1" t="s">
-        <v>144</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>343</v>
-      </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>158</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>159</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.3">
@@ -2448,28 +2448,28 @@
         <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J2" t="s">
+        <v>242</v>
+      </c>
+      <c r="K2" t="s">
         <v>243</v>
       </c>
-      <c r="K2" t="s">
-        <v>244</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -2514,31 +2514,31 @@
         <v>1</v>
       </c>
       <c r="AE2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AF2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AG2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH2" t="s">
         <v>243</v>
       </c>
-      <c r="AH2" t="s">
-        <v>244</v>
-      </c>
       <c r="AI2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL2">
         <v>1</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN2">
         <v>1</v>
@@ -2577,31 +2577,31 @@
         <v>0</v>
       </c>
       <c r="AZ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="BB2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC2" t="s">
         <v>273</v>
       </c>
-      <c r="BC2" t="s">
-        <v>274</v>
-      </c>
       <c r="BD2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BE2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BF2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BG2">
         <v>1</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI2">
         <v>1</v>
@@ -2666,28 +2666,28 @@
         <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J3" t="s">
+        <v>242</v>
+      </c>
+      <c r="K3" t="s">
         <v>243</v>
       </c>
-      <c r="K3" t="s">
-        <v>244</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -2732,31 +2732,31 @@
         <v>1</v>
       </c>
       <c r="AE3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AF3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AG3" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH3" t="s">
         <v>243</v>
       </c>
-      <c r="AH3" t="s">
-        <v>244</v>
-      </c>
       <c r="AI3" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL3">
         <v>1</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN3">
         <v>1</v>
@@ -2795,31 +2795,31 @@
         <v>0</v>
       </c>
       <c r="AZ3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="BB3" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC3" t="s">
         <v>273</v>
       </c>
-      <c r="BC3" t="s">
-        <v>274</v>
-      </c>
       <c r="BD3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BE3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BF3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BG3">
         <v>1</v>
       </c>
       <c r="BH3" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI3">
         <v>1</v>
@@ -2884,28 +2884,28 @@
         <v>73</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J4" t="s">
+        <v>242</v>
+      </c>
+      <c r="K4" t="s">
         <v>243</v>
       </c>
-      <c r="K4" t="s">
-        <v>244</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -2950,31 +2950,31 @@
         <v>0</v>
       </c>
       <c r="AE4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AF4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AG4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AH4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AI4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AJ4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL4">
         <v>1</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AN4">
         <v>1</v>
@@ -3013,31 +3013,31 @@
         <v>0</v>
       </c>
       <c r="AZ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="BB4" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC4" t="s">
         <v>273</v>
       </c>
-      <c r="BC4" t="s">
-        <v>274</v>
-      </c>
       <c r="BD4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BE4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BF4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BG4">
         <v>1</v>
       </c>
       <c r="BH4" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI4">
         <v>1</v>
@@ -3102,28 +3102,28 @@
         <v>77</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K5" t="s">
         <v>243</v>
       </c>
-      <c r="K5" t="s">
-        <v>244</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -3168,31 +3168,31 @@
         <v>1</v>
       </c>
       <c r="AE5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="AF5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AG5" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH5" t="s">
         <v>243</v>
       </c>
-      <c r="AH5" t="s">
-        <v>244</v>
-      </c>
       <c r="AI5" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL5">
         <v>1</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN5">
         <v>1</v>
@@ -3231,31 +3231,31 @@
         <v>0</v>
       </c>
       <c r="AZ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA5" t="s">
+        <v>271</v>
+      </c>
+      <c r="BB5" t="s">
         <v>272</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BC5" t="s">
         <v>273</v>
       </c>
-      <c r="BC5" t="s">
-        <v>274</v>
-      </c>
       <c r="BD5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BE5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BF5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BG5">
         <v>1</v>
       </c>
       <c r="BH5" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI5">
         <v>1</v>
@@ -3320,28 +3320,28 @@
         <v>78</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J6" t="s">
+        <v>242</v>
+      </c>
+      <c r="K6" t="s">
         <v>243</v>
       </c>
-      <c r="K6" t="s">
-        <v>244</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -3386,31 +3386,31 @@
         <v>1</v>
       </c>
       <c r="AE6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AF6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AG6" t="s">
+        <v>242</v>
+      </c>
+      <c r="AH6" t="s">
         <v>243</v>
       </c>
-      <c r="AH6" t="s">
-        <v>244</v>
-      </c>
       <c r="AI6" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL6">
         <v>1</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN6">
         <v>1</v>
@@ -3449,31 +3449,31 @@
         <v>0</v>
       </c>
       <c r="AZ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="BB6" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC6" t="s">
         <v>273</v>
       </c>
-      <c r="BC6" t="s">
-        <v>274</v>
-      </c>
       <c r="BD6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BE6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BF6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BG6">
         <v>1</v>
       </c>
       <c r="BH6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI6">
         <v>1</v>
@@ -3538,13 +3538,13 @@
         <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M7" t="s">
         <v>9</v>
@@ -3556,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -3601,16 +3601,16 @@
         <v>1</v>
       </c>
       <c r="AE7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="AF7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AG7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ7" t="s">
         <v>9</v>
@@ -3622,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN7">
         <v>0</v>
@@ -3661,31 +3661,31 @@
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="BB7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="BC7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="BD7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BE7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BF7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BG7">
         <v>1</v>
       </c>
       <c r="BH7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BI7">
         <v>1</v>
@@ -3750,13 +3750,13 @@
         <v>84</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M8" t="s">
         <v>9</v>
@@ -3768,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -3813,16 +3813,16 @@
         <v>1</v>
       </c>
       <c r="AE8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AF8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AG8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ8" t="s">
         <v>9</v>
@@ -3834,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="AM8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN8">
         <v>0</v>
@@ -3873,31 +3873,31 @@
         <v>0</v>
       </c>
       <c r="AZ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA8" t="s">
+        <v>278</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>280</v>
+      </c>
+      <c r="BC8" t="s">
         <v>279</v>
       </c>
-      <c r="BB8" t="s">
-        <v>281</v>
-      </c>
-      <c r="BC8" t="s">
-        <v>280</v>
-      </c>
       <c r="BD8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BE8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BF8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BG8">
         <v>1</v>
       </c>
       <c r="BH8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BI8">
         <v>1</v>
@@ -3962,25 +3962,25 @@
         <v>85</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -4025,28 +4025,28 @@
         <v>1</v>
       </c>
       <c r="AE9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AF9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AG9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AJ9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL9">
         <v>1</v>
       </c>
       <c r="AM9" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN9">
         <v>0</v>
@@ -4085,31 +4085,31 @@
         <v>0</v>
       </c>
       <c r="AZ9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="BB9" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC9" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="BC9" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="BD9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BE9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG9">
         <v>1</v>
       </c>
       <c r="BH9" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI9">
         <v>1</v>
@@ -4171,28 +4171,28 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -4237,28 +4237,28 @@
         <v>1</v>
       </c>
       <c r="AE10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="AF10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL10">
         <v>1</v>
       </c>
       <c r="AM10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN10">
         <v>0</v>
@@ -4297,31 +4297,31 @@
         <v>0</v>
       </c>
       <c r="AZ10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="BB10" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC10" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="BC10" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="BD10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BE10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG10">
         <v>1</v>
       </c>
       <c r="BH10" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI10">
         <v>1</v>
@@ -4386,25 +4386,25 @@
         <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -4449,28 +4449,28 @@
         <v>1</v>
       </c>
       <c r="AE11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AF11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AJ11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL11">
         <v>1</v>
       </c>
       <c r="AM11" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AN11">
         <v>0</v>
@@ -4509,31 +4509,31 @@
         <v>0</v>
       </c>
       <c r="AZ11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA11" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB11" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="BB11" s="3" t="s">
+      <c r="BC11" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="BC11" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="BD11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BE11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG11">
         <v>1</v>
       </c>
       <c r="BH11" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI11">
         <v>1</v>
@@ -4598,28 +4598,28 @@
         <v>89</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O12">
         <v>1</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -4664,31 +4664,31 @@
         <v>1</v>
       </c>
       <c r="AE12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AF12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AH12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AI12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AJ12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL12">
         <v>1</v>
       </c>
       <c r="AM12" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN12">
         <v>1</v>
@@ -4727,31 +4727,31 @@
         <v>0</v>
       </c>
       <c r="AZ12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BB12" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC12" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="BC12" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="BD12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BE12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG12">
         <v>1</v>
       </c>
       <c r="BH12" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI12">
         <v>1</v>
@@ -4816,28 +4816,28 @@
         <v>74</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K13" t="s">
         <v>251</v>
       </c>
-      <c r="K13" t="s">
-        <v>252</v>
-      </c>
       <c r="L13" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -4882,31 +4882,31 @@
         <v>1</v>
       </c>
       <c r="AE13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="AF13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AG13" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH13" t="s">
         <v>251</v>
       </c>
-      <c r="AH13" t="s">
-        <v>252</v>
-      </c>
       <c r="AI13" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AJ13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL13">
         <v>1</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN13">
         <v>1</v>
@@ -4945,31 +4945,31 @@
         <v>0</v>
       </c>
       <c r="AZ13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BB13" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC13" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="BC13" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="BD13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BE13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG13">
         <v>1</v>
       </c>
       <c r="BH13" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI13">
         <v>1</v>
@@ -5034,28 +5034,28 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -5100,31 +5100,31 @@
         <v>0</v>
       </c>
       <c r="AE14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="AF14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AH14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL14">
         <v>1</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN14">
         <v>1</v>
@@ -5163,31 +5163,31 @@
         <v>0</v>
       </c>
       <c r="AZ14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA14" t="s">
+        <v>289</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>252</v>
+      </c>
+      <c r="BC14" t="s">
         <v>290</v>
       </c>
-      <c r="BB14" t="s">
-        <v>253</v>
-      </c>
-      <c r="BC14" t="s">
-        <v>291</v>
-      </c>
       <c r="BD14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BE14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BF14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BG14">
         <v>1</v>
       </c>
       <c r="BH14" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI14">
         <v>1</v>
@@ -5252,28 +5252,28 @@
         <v>91</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q15">
         <v>1</v>
@@ -5318,31 +5318,31 @@
         <v>0</v>
       </c>
       <c r="AE15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AF15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AH15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK15" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL15">
         <v>1</v>
       </c>
       <c r="AM15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN15">
         <v>1</v>
@@ -5381,31 +5381,31 @@
         <v>0</v>
       </c>
       <c r="AZ15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BB15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BC15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BD15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BE15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BF15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="BG15">
         <v>1</v>
       </c>
       <c r="BH15" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI15">
         <v>1</v>
@@ -5470,25 +5470,25 @@
         <v>90</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -5533,31 +5533,31 @@
         <v>0</v>
       </c>
       <c r="AE16" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AF16" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="AH16" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AJ16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AL16">
         <v>1</v>
       </c>
       <c r="AM16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AN16">
         <v>1</v>
@@ -5596,28 +5596,28 @@
         <v>0</v>
       </c>
       <c r="AZ16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="BB16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="BD16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BE16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG16">
         <v>1</v>
       </c>
       <c r="BH16" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="BI16">
         <v>1</v>
@@ -5682,28 +5682,28 @@
         <v>92</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q17">
         <v>1</v>
@@ -5748,31 +5748,31 @@
         <v>0</v>
       </c>
       <c r="AE17" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="AF17" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="AG17" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AH17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AJ17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK17" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL17">
         <v>1</v>
       </c>
       <c r="AM17" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AN17">
         <v>1</v>
@@ -5811,28 +5811,28 @@
         <v>0</v>
       </c>
       <c r="AZ17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA17" t="s">
+        <v>303</v>
+      </c>
+      <c r="BB17" t="s">
         <v>304</v>
       </c>
-      <c r="BB17" t="s">
-        <v>305</v>
-      </c>
       <c r="BD17" t="s">
+        <v>337</v>
+      </c>
+      <c r="BE17" t="s">
         <v>338</v>
       </c>
-      <c r="BE17" t="s">
-        <v>339</v>
-      </c>
       <c r="BF17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="BG17">
         <v>1</v>
       </c>
       <c r="BH17" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="BI17">
         <v>0</v>
@@ -5897,25 +5897,25 @@
         <v>93</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -5960,28 +5960,28 @@
         <v>1</v>
       </c>
       <c r="AE18" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AF18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AG18" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL18">
         <v>1</v>
       </c>
       <c r="AM18" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN18">
         <v>0</v>
@@ -6020,31 +6020,31 @@
         <v>0</v>
       </c>
       <c r="AZ18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="BB18" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC18" t="s">
         <v>284</v>
       </c>
-      <c r="BC18" t="s">
-        <v>285</v>
-      </c>
       <c r="BD18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BE18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG18">
         <v>1</v>
       </c>
       <c r="BH18" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI18">
         <v>1</v>
@@ -6109,25 +6109,25 @@
         <v>66</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -6172,28 +6172,28 @@
         <v>1</v>
       </c>
       <c r="AE19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AF19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="AG19" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK19" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL19">
         <v>1</v>
       </c>
       <c r="AM19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN19">
         <v>0</v>
@@ -6232,31 +6232,31 @@
         <v>0</v>
       </c>
       <c r="AZ19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="BB19" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC19" t="s">
         <v>284</v>
       </c>
-      <c r="BC19" t="s">
-        <v>285</v>
-      </c>
       <c r="BD19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BE19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG19">
         <v>1</v>
       </c>
       <c r="BH19" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI19">
         <v>1</v>
@@ -6321,25 +6321,25 @@
         <v>67</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -6384,28 +6384,28 @@
         <v>1</v>
       </c>
       <c r="AE20" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="AF20" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="AG20" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK20" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL20">
         <v>1</v>
       </c>
       <c r="AM20" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN20">
         <v>0</v>
@@ -6444,31 +6444,31 @@
         <v>0</v>
       </c>
       <c r="AZ20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="BB20" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC20" t="s">
         <v>284</v>
       </c>
-      <c r="BC20" t="s">
-        <v>285</v>
-      </c>
       <c r="BD20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BE20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BF20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="BG20">
         <v>1</v>
       </c>
       <c r="BH20" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI20">
         <v>1</v>
@@ -6533,28 +6533,28 @@
         <v>94</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="K21" t="s">
         <v>261</v>
       </c>
-      <c r="K21" t="s">
-        <v>262</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O21">
         <v>1</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q21">
         <v>1</v>
@@ -6599,31 +6599,31 @@
         <v>0</v>
       </c>
       <c r="AE21" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AF21" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AG21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AH21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AJ21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AK21" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AL21">
         <v>1</v>
       </c>
       <c r="AM21" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AN21">
         <v>1</v>
@@ -6662,31 +6662,31 @@
         <v>0</v>
       </c>
       <c r="AZ21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="BB21" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC21" t="s">
         <v>273</v>
       </c>
-      <c r="BC21" t="s">
-        <v>274</v>
-      </c>
       <c r="BD21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="BE21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BF21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="BG21">
         <v>1</v>
       </c>
       <c r="BH21" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="BI21">
         <v>1</v>
@@ -6751,28 +6751,28 @@
         <v>83</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O22">
         <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q22">
         <v>1</v>
@@ -6817,31 +6817,31 @@
         <v>0</v>
       </c>
       <c r="AE22" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AF22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AG22" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AH22" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AJ22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AL22">
         <v>1</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AN22">
         <v>1</v>
@@ -6880,31 +6880,31 @@
         <v>1</v>
       </c>
       <c r="AZ22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA22" t="s">
+        <v>299</v>
+      </c>
+      <c r="BB22" t="s">
+        <v>302</v>
+      </c>
+      <c r="BC22" t="s">
         <v>300</v>
       </c>
-      <c r="BB22" t="s">
-        <v>303</v>
-      </c>
-      <c r="BC22" t="s">
-        <v>301</v>
-      </c>
       <c r="BD22" t="s">
+        <v>324</v>
+      </c>
+      <c r="BE22" t="s">
         <v>325</v>
       </c>
-      <c r="BE22" t="s">
-        <v>326</v>
-      </c>
       <c r="BF22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="BG22">
         <v>1</v>
       </c>
       <c r="BH22" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BI22">
         <v>1</v>
@@ -6969,25 +6969,25 @@
         <v>88</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O23">
         <v>1</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -7032,31 +7032,31 @@
         <v>1</v>
       </c>
       <c r="AE23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AF23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="AG23" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AH23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK23" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL23">
         <v>1</v>
       </c>
       <c r="AM23" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN23">
         <v>0</v>
@@ -7095,28 +7095,28 @@
         <v>0</v>
       </c>
       <c r="AZ23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="BB23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="BD23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="BE23" t="s">
+        <v>319</v>
+      </c>
+      <c r="BF23" t="s">
+        <v>319</v>
+      </c>
+      <c r="BG23">
+        <v>1</v>
+      </c>
+      <c r="BH23" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="BF23" t="s">
-        <v>320</v>
-      </c>
-      <c r="BG23">
-        <v>1</v>
-      </c>
-      <c r="BH23" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="BI23">
         <v>0</v>
@@ -7181,25 +7181,25 @@
         <v>82</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O24">
         <v>1</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -7244,28 +7244,28 @@
         <v>1</v>
       </c>
       <c r="AE24" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AF24" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AG24" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL24">
         <v>1</v>
       </c>
       <c r="AM24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN24">
         <v>0</v>
@@ -7304,28 +7304,28 @@
         <v>0</v>
       </c>
       <c r="AZ24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="BB24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BD24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="BE24" t="s">
+        <v>319</v>
+      </c>
+      <c r="BF24" t="s">
+        <v>319</v>
+      </c>
+      <c r="BG24">
+        <v>1</v>
+      </c>
+      <c r="BH24" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="BF24" t="s">
-        <v>320</v>
-      </c>
-      <c r="BG24">
-        <v>1</v>
-      </c>
-      <c r="BH24" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="BI24">
         <v>0</v>
@@ -7390,25 +7390,25 @@
         <v>68</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O25">
         <v>1</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -7453,28 +7453,28 @@
         <v>1</v>
       </c>
       <c r="AE25" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AF25" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AL25">
         <v>1</v>
       </c>
       <c r="AM25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN25">
         <v>0</v>
@@ -7513,28 +7513,28 @@
         <v>0</v>
       </c>
       <c r="AZ25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="BB25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BD25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="BE25" t="s">
+        <v>319</v>
+      </c>
+      <c r="BF25" t="s">
+        <v>319</v>
+      </c>
+      <c r="BG25">
+        <v>1</v>
+      </c>
+      <c r="BH25" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="BF25" t="s">
-        <v>320</v>
-      </c>
-      <c r="BG25">
-        <v>1</v>
-      </c>
-      <c r="BH25" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="BI25">
         <v>0</v>
@@ -7599,25 +7599,25 @@
         <v>75</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L26" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="M26" t="s">
         <v>371</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="O26">
         <v>1</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -7662,28 +7662,28 @@
         <v>1</v>
       </c>
       <c r="AE26" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AF26" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="AG26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AI26" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="AJ26" t="s">
         <v>371</v>
       </c>
-      <c r="AJ26" t="s">
+      <c r="AK26" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="AK26" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="AL26">
         <v>1</v>
       </c>
       <c r="AM26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN26">
         <v>0</v>
@@ -7722,28 +7722,28 @@
         <v>0</v>
       </c>
       <c r="AZ26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="BB26" t="s">
+        <v>313</v>
+      </c>
+      <c r="BD26" t="s">
         <v>314</v>
       </c>
-      <c r="BD26" t="s">
-        <v>315</v>
-      </c>
       <c r="BE26" t="s">
+        <v>319</v>
+      </c>
+      <c r="BF26" t="s">
+        <v>319</v>
+      </c>
+      <c r="BG26">
+        <v>1</v>
+      </c>
+      <c r="BH26" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="BF26" t="s">
-        <v>320</v>
-      </c>
-      <c r="BG26">
-        <v>1</v>
-      </c>
-      <c r="BH26" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="BI26">
         <v>0</v>
@@ -7808,25 +7808,25 @@
         <v>80</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O27">
         <v>1</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -7871,28 +7871,28 @@
         <v>1</v>
       </c>
       <c r="AE27" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AF27" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AG27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AI27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AK27" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AL27">
         <v>1</v>
       </c>
       <c r="AM27" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AN27">
         <v>0</v>
@@ -7931,28 +7931,28 @@
         <v>0</v>
       </c>
       <c r="AZ27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="BB27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BD27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="BE27" t="s">
+        <v>319</v>
+      </c>
+      <c r="BF27" t="s">
+        <v>319</v>
+      </c>
+      <c r="BG27">
+        <v>1</v>
+      </c>
+      <c r="BH27" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="BF27" t="s">
-        <v>320</v>
-      </c>
-      <c r="BG27">
-        <v>1</v>
-      </c>
-      <c r="BH27" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="BI27">
         <v>0</v>
@@ -8014,28 +8014,28 @@
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="O28">
         <v>1</v>
       </c>
       <c r="P28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -8080,29 +8080,29 @@
         <v>1</v>
       </c>
       <c r="AE28" t="s">
-        <v>135</v>
+        <v>457</v>
       </c>
       <c r="AF28" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AG28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AH28" s="1"/>
       <c r="AI28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AJ28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AK28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AL28">
         <v>1</v>
       </c>
       <c r="AM28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AN28">
         <v>0</v>
@@ -8141,28 +8141,28 @@
         <v>0</v>
       </c>
       <c r="AZ28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA28" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="BB28" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD28" t="s">
         <v>182</v>
       </c>
-      <c r="BD28" t="s">
-        <v>183</v>
-      </c>
       <c r="BE28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="BF28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="BG28">
         <v>1</v>
       </c>
       <c r="BH28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BI28">
         <v>0</v>
@@ -8227,28 +8227,28 @@
         <v>81</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K29" t="s">
         <v>258</v>
       </c>
-      <c r="K29" t="s">
-        <v>259</v>
-      </c>
       <c r="L29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="O29">
         <v>1</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -8293,28 +8293,28 @@
         <v>0</v>
       </c>
       <c r="AE29" t="s">
-        <v>379</v>
+        <v>458</v>
       </c>
       <c r="AF29" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="AG29" t="s">
+        <v>378</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>182</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>316</v>
+      </c>
+      <c r="AK29" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL29">
+        <v>1</v>
+      </c>
+      <c r="AM29" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="AI29" t="s">
-        <v>183</v>
-      </c>
-      <c r="AJ29" t="s">
-        <v>317</v>
-      </c>
-      <c r="AK29" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="AL29">
-        <v>1</v>
-      </c>
-      <c r="AM29" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="AN29">
         <v>0</v>
@@ -8353,28 +8353,28 @@
         <v>0</v>
       </c>
       <c r="AZ29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA29" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="BB29" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD29" t="s">
         <v>182</v>
       </c>
-      <c r="BD29" t="s">
-        <v>183</v>
-      </c>
       <c r="BE29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="BF29" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="BG29">
         <v>1</v>
       </c>
       <c r="BH29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BI29">
         <v>0</v>
@@ -8529,8 +8529,8 @@
     <cfRule type="duplicateValues" dxfId="49" priority="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K31 K34:K1048576">
+    <cfRule type="top10" priority="103" percent="1" rank="10"/>
     <cfRule type="duplicateValues" dxfId="48" priority="102"/>
-    <cfRule type="top10" priority="103" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K13 K16:K29">
     <cfRule type="duplicateValues" dxfId="47" priority="117"/>
@@ -8656,34 +8656,34 @@
     <cfRule type="duplicateValues" dxfId="33" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2:AH3">
+    <cfRule type="top10" priority="69" percent="1" rank="10"/>
     <cfRule type="duplicateValues" dxfId="32" priority="68"/>
-    <cfRule type="top10" priority="69" percent="1" rank="10"/>
     <cfRule type="duplicateValues" dxfId="31" priority="70"/>
     <cfRule type="duplicateValues" dxfId="30" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH5:AH6">
-    <cfRule type="duplicateValues" dxfId="29" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="61"/>
     <cfRule type="top10" priority="60" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="61"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH7:AH8">
     <cfRule type="duplicateValues" dxfId="26" priority="50"/>
     <cfRule type="top10" priority="51" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH9:AH13">
-    <cfRule type="duplicateValues" dxfId="23" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="43"/>
     <cfRule type="top10" priority="42" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="41"/>
     <cfRule type="duplicateValues" dxfId="21" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH14">
-    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
     <cfRule type="top10" priority="17" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -8708,16 +8708,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH18:AH20">
-    <cfRule type="duplicateValues" dxfId="14" priority="32"/>
     <cfRule type="top10" priority="33" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH25">
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="25"/>
     <cfRule type="top10" priority="24" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH26">
     <cfRule type="duplicateValues" dxfId="8" priority="77"/>
@@ -9179,7 +9179,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AW2:AZ13 AW16:AZ29 AX14:AZ15">
+  <conditionalFormatting sqref="AW16:AY29 AX14:AY15 AW2:AZ5 AW6:AY13 AZ6:AZ29">
     <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -9332,6 +9332,7 @@
     <hyperlink ref="AF25" r:id="rId92" xr:uid="{DF10C723-F06F-42D2-BBC2-631BB4973626}"/>
     <hyperlink ref="AF19" r:id="rId93" xr:uid="{70A5BAAA-5790-4919-8346-E017C3255984}"/>
     <hyperlink ref="AF14" r:id="rId94" xr:uid="{9129E375-E5C7-43F9-AB82-3C6F6638EBD4}"/>
+    <hyperlink ref="AE29" r:id="rId95" xr:uid="{952A0304-5B2C-4D4B-BA4A-D4C03F0B7612}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9349,147 +9350,147 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" t="s">
         <v>327</v>
-      </c>
-      <c r="C2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" t="s">
         <v>188</v>
       </c>
-      <c r="B3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C3" t="s">
-        <v>189</v>
-      </c>
       <c r="D3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" t="s">
         <v>323</v>
       </c>
-      <c r="B5" t="s">
-        <v>322</v>
-      </c>
-      <c r="C5" t="s">
-        <v>324</v>
-      </c>
       <c r="D5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
         <v>330</v>
       </c>
-      <c r="B6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C6" t="s">
-        <v>331</v>
-      </c>
       <c r="D6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" t="s">
         <v>334</v>
       </c>
-      <c r="C7" t="s">
-        <v>335</v>
-      </c>
       <c r="D7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" t="s">
         <v>339</v>
       </c>
-      <c r="C8" t="s">
-        <v>340</v>
-      </c>
       <c r="D8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" t="s">
         <v>346</v>
       </c>
-      <c r="B9" t="s">
-        <v>348</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>347</v>
-      </c>
-      <c r="D9" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B10" t="s">
         <v>354</v>
       </c>
-      <c r="B10" t="s">
-        <v>355</v>
-      </c>
       <c r="C10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" t="s">
         <v>180</v>
       </c>
-      <c r="B11" t="s">
-        <v>358</v>
-      </c>
-      <c r="C11" t="s">
-        <v>181</v>
-      </c>
       <c r="D11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -9497,69 +9498,69 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D13" t="s">
         <v>363</v>
-      </c>
-      <c r="D13" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C14" t="s">
+        <v>365</v>
+      </c>
+      <c r="D14" t="s">
         <v>366</v>
-      </c>
-      <c r="D14" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B16" t="s">
+        <v>373</v>
+      </c>
+      <c r="C16" t="s">
         <v>374</v>
       </c>
-      <c r="C16" t="s">
-        <v>375</v>
-      </c>
       <c r="D16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" t="s">
         <v>145</v>
-      </c>
-      <c r="C18" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -10302,7 +10303,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -10337,212 +10338,212 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81" t="s">
         <v>213</v>
-      </c>
-      <c r="B81" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
+        <v>232</v>
+      </c>
+      <c r="C82" t="s">
+        <v>218</v>
+      </c>
+      <c r="D82" t="s">
         <v>233</v>
-      </c>
-      <c r="C82" t="s">
-        <v>219</v>
-      </c>
-      <c r="D82" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>214</v>
+      </c>
+      <c r="B83" t="s">
         <v>215</v>
-      </c>
-      <c r="B83" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
+        <v>219</v>
+      </c>
+      <c r="C86" t="s">
         <v>220</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>221</v>
       </c>
-      <c r="D86" t="s">
-        <v>222</v>
-      </c>
       <c r="E86" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C91">
         <v>33480</v>
       </c>
       <c r="E91" t="s">
+        <v>227</v>
+      </c>
+      <c r="F91" t="s">
         <v>228</v>
-      </c>
-      <c r="F91" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
+        <v>237</v>
+      </c>
+      <c r="F92" t="s">
         <v>238</v>
-      </c>
-      <c r="F92" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>204</v>
+      </c>
+      <c r="B95" t="s">
         <v>205</v>
-      </c>
-      <c r="B95" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>207</v>
+      </c>
+      <c r="B97" t="s">
         <v>208</v>
-      </c>
-      <c r="B97" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>210</v>
+      </c>
+      <c r="B99" t="s">
         <v>211</v>
-      </c>
-      <c r="B99" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change in data and file
</commit_message>
<xml_diff>
--- a/data_health_insurance.xlsx
+++ b/data_health_insurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marij\PycharmProjects\health_insurance_cloud_networking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9583B5-6C1B-461D-B106-BDDED764EA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466BD0A1-48B8-4008-933F-675F53FE6502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="459">
   <si>
     <t>Company</t>
   </si>
@@ -848,574 +848,574 @@
     <t>apps.zorgenzekerheid.nl</t>
   </si>
   <si>
+    <t>13.248.206.174;76.223.71.132</t>
+  </si>
+  <si>
+    <t>2600:9000:a61c:a0a1:422:c6a5:8963:492c;2600:9000:a50f:9f2b:9243:9933:1f8c:a16c</t>
+  </si>
+  <si>
+    <t>Check mijnzorg.fbto.nl where client see informations</t>
+  </si>
+  <si>
+    <t>2a02:26f0:c900:b::5f65:4a0c;2a02:26f0:c900:b::5f65:4a2c</t>
+  </si>
+  <si>
+    <t>2.18.244.78;2.18.244.78</t>
+  </si>
+  <si>
+    <t>104.16.146.28;104.16.147.28</t>
+  </si>
+  <si>
+    <t>2606:4700::6810:921c;2606:4700::6810:931c</t>
+  </si>
+  <si>
+    <t>Login ISP</t>
+  </si>
+  <si>
+    <t>Login cloud</t>
+  </si>
+  <si>
+    <t>2a02:26f0:c900:b::5f65:4a13;2a02:26f0:c900:b::5f65:4a32</t>
+  </si>
+  <si>
+    <t>Support iDIN</t>
+  </si>
+  <si>
+    <t>2603:1026:3000:148::7;2603:1026:3000:148::10;2603:1026:3000:150::a;2603:1026:3000:148::e;2603:1026:3000:150::5;2603:1026:3000:150::6;2603:1027:1:158::8;2603:1026:3000:150::8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t>20.190.160.17;20.190.160.22;40.126.32.76;40.126.32.136;20.190.160.14;40.126.32.140;40.126.32.68;40.126.32.74</t>
+  </si>
+  <si>
+    <t>109.68.90.49</t>
+  </si>
+  <si>
+    <t>141.193.179.212</t>
+  </si>
+  <si>
+    <t>141.193.179.165</t>
+  </si>
+  <si>
+    <t>inloggen.vgz.nl</t>
+  </si>
+  <si>
+    <t>Support login</t>
+  </si>
+  <si>
+    <t>64.113.50.231</t>
+  </si>
+  <si>
+    <t>141.193.179.238</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>ManagedWay</t>
+  </si>
+  <si>
+    <t>KPN</t>
+  </si>
+  <si>
+    <t>AS53292 ManagedWay;ManagedWay (managedway.com);ManagedWay;MWAY</t>
+  </si>
+  <si>
+    <t>ManagedWay;MWAY</t>
+  </si>
+  <si>
+    <t>MWAY</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft </t>
+  </si>
+  <si>
+    <t>Microsoft Corporation</t>
+  </si>
+  <si>
+    <t>AS8075 Microsoft Corporation;Microsoft Corporation;Microsoft Corporation (microsoft.com)</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Amazon.com Inc.;Amazon.com, Inc.;AMAZON-02</t>
+  </si>
+  <si>
+    <t>AS16509 Amazon.com, Inc.;Amazon.com, Inc. (aws.com);AMAZON-02</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>CloudFlare</t>
+  </si>
+  <si>
+    <t>Cloudflare</t>
+  </si>
+  <si>
+    <t>AS13335 Cloudflare, Inc.;Cloudflare, Inc.;CLOUDFLARENET</t>
+  </si>
+  <si>
+    <t>CloudFlare Inc.;CLOUDFLARENET;Cloudflare</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>AS25148 ORANGE BUSINESS DIGITAL NORWAY AS;Signicat Vips</t>
+  </si>
+  <si>
+    <t>Orange Business Digital Norway AS;ORANGE BUSINESS DIGITAL NORWAY AS;Orange Business NO Network;ORANGE BUSINESS DIGITAL NORWAY AS;Basefarm Webdeal network</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Login Europa</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>Akamai Technologies Inc.; Akamai International B.V.</t>
+  </si>
+  <si>
+    <t>AS20940 Akamai International B.V.;Akamai Technologies, Inc.;Akamai Technologies, Inc. (akamai.com);Akamai International B.V.</t>
+  </si>
+  <si>
+    <t>Akamai</t>
+  </si>
+  <si>
+    <t>San Jose</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Home Location IP</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>A100 ROW GmbH</t>
+  </si>
+  <si>
+    <t>A100 ROW GmbH;Amazon.com Inc.;Amazon.com, Inc.;AMAZON-02</t>
+  </si>
+  <si>
+    <t>Amazon germany</t>
+  </si>
+  <si>
+    <t>Amazone</t>
+  </si>
+  <si>
+    <t>Home in Europa</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>ASR Nederland N.V.;Asr Nederland N.V.;ASR Nederland N.V.</t>
+  </si>
+  <si>
+    <t>AS50737 ASR Nederland N.V.; Asr Nederland N.V. (asr.nl); ASR Nederland N.V.</t>
+  </si>
+  <si>
+    <t>Tilburg</t>
+  </si>
+  <si>
+    <t>AS1136 KPN B.V.;Cz Groep Zorgverzekeringen (kpn.net);KPN B.V.</t>
+  </si>
+  <si>
+    <t>KPN CZ</t>
+  </si>
+  <si>
+    <t>KPN B.V.</t>
+  </si>
+  <si>
+    <t>AS16625 Akamai Technologies, Inc.</t>
+  </si>
+  <si>
+    <t>Akamai Amsterdam</t>
+  </si>
+  <si>
+    <t>Akamai Technologies, Inc.</t>
+  </si>
+  <si>
+    <t>AS9150 Interconnect;ML Consultancy;Indicia e-Business B.V.</t>
+  </si>
+  <si>
+    <t>Indicia e-Business B.V.; MLC/InterConnect; Ml Consultancy; MLC/InterConnect routed block</t>
+  </si>
+  <si>
+    <t>s-Hertogenbosch</t>
+  </si>
+  <si>
+    <t>Interconnect</t>
+  </si>
+  <si>
+    <t>interconnect</t>
+  </si>
+  <si>
+    <t>Claranet</t>
+  </si>
+  <si>
+    <t>AS8426 Claranet Limited;UnitedConsumers Brand &amp; IP B.V;Unitedconsumers Brand &amp; Ip B.V. (unitedconsumers.com)</t>
+  </si>
+  <si>
+    <t>UnitedConsumers Brand &amp; IP B.V.;Claranet Limited</t>
+  </si>
+  <si>
+    <t>Registration europa</t>
+  </si>
+  <si>
+    <t>Registration IPv4</t>
+  </si>
+  <si>
+    <t>193.173.52.131</t>
+  </si>
+  <si>
+    <t>Registration Location</t>
+  </si>
+  <si>
+    <t>Netherlandse</t>
+  </si>
+  <si>
+    <t>https://www.unitedconsumers.com/zorgverzekering/aanmelden/offerte.asp</t>
+  </si>
+  <si>
+    <t>https://www.zekur.nl/zorgverzekering/afsluiten</t>
+  </si>
+  <si>
+    <t>https://www.defriesland.nl/zorgverzekering/premie-berekenen/persoonsgegevens</t>
+  </si>
+  <si>
+    <t>https://www.fbto.nl/zorgverzekering/premie-berekenen/naam</t>
+  </si>
+  <si>
+    <t>https://bankieren.rabobank.nl/</t>
+  </si>
+  <si>
+    <t>https://www.dechristelijkezorgverzekeraar.nl/zorgverzekering/premie-berekenen/persoonsgegevens</t>
+  </si>
+  <si>
+    <t>https://www.zilverenkruis.nl/consumenten/zorgverzekering/premie-berekenen/persoonsgegevens</t>
+  </si>
+  <si>
+    <t>https://www.asr.nl/verzekeringen/zorgverzekering/afsluiten#/user-data</t>
+  </si>
+  <si>
+    <t>https://www.asr.nl/verzekeringen/zorgverzekering/ikkieszelf/afsluiten#/user-data</t>
+  </si>
+  <si>
+    <t>https://www.cz.nl/zorgverzekering/premie-berekenen/aanmelden</t>
+  </si>
+  <si>
+    <t>https://www.just.nl/zorgverzekering/premie-berekenen/aanmelden</t>
+  </si>
+  <si>
+    <t>https://www.czdirect.cz.nl/zorgverzekering/premie-berekenen/aanmelden</t>
+  </si>
+  <si>
+    <t>https://www.nn.nl/Particulier/Zorgverzekering/Zorgverzekering-aanvragen.htm#aanvrager</t>
+  </si>
+  <si>
+    <t>https://www.ohra.nl/zorgverzekering/berekenen#aanvrager</t>
+  </si>
+  <si>
+    <t>https://aanmelden.dsw.nl/aanmelden</t>
+  </si>
+  <si>
+    <t>https://aanmelden.stadholland.nl/</t>
+  </si>
+  <si>
+    <t>Registration traditioneel</t>
+  </si>
+  <si>
+    <t>https://aanvraag.salland.nl/persoonsgegevens</t>
+  </si>
+  <si>
+    <t>https://aanvragen.aevitae.com/nl/44086/personal_data</t>
+  </si>
+  <si>
+    <t>https://www.anderzorg.nl/premie-berekenen-en-aanvragen</t>
+  </si>
+  <si>
+    <t>https://www.menzis.nl/premie-berekenen-en-aanvragen</t>
+  </si>
+  <si>
+    <t>https://www.vinkvink.nl/premie-berekenen-en-aanvragen</t>
+  </si>
+  <si>
+    <t>https://aanvragen.onvz.nl/index.html</t>
+  </si>
+  <si>
+    <t>https://aanvragen.vvaazorgverzekering.nl/index.html</t>
+  </si>
+  <si>
+    <t>https://www.vgzbewuzt.nl/premie-berekenen/stap4</t>
+  </si>
+  <si>
+    <t>https://www.vgz.nl/zorgverzekering/premie-berekenen-en-afsluiten#/stap2</t>
+  </si>
+  <si>
+    <t>https://www.unive.nl/verzekeringspakket/premieberekenen-en-afsluiten/Gegevens?AanvraagId=54542</t>
+  </si>
+  <si>
+    <t>Registration vs Home</t>
+  </si>
+  <si>
+    <t>Login vs Home</t>
+  </si>
+  <si>
+    <t>13.107.246.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2620:1ec:bdf::67</t>
+  </si>
+  <si>
+    <t>141.101.90.104;141.101.90.105;141.101.90.106;141.101.90.107</t>
+  </si>
+  <si>
+    <t>2a06:98c1:3200::90:80;2a06:98c1:3200::90:81;2a06:98c1:3200::90:82;2a06:98c1:3200::90:83</t>
+  </si>
+  <si>
+    <t>2a05:d014:145:aa02:39cc:ca87:679c:1a44;2a05:d014:145:aa01:e7ed:1bdf:317c:168e;2a05:d014:145:aa00:63e4:ad8e:c1c7:8675</t>
+  </si>
+  <si>
+    <t>3.125.189.196;3.126.216.110;3.127.11.115</t>
+  </si>
+  <si>
+    <t>2a02:26f0:c900:b::5f65:4a23;2a02:26f0:c900:b::5f65:4a27;2a02:26f0:c900:b::5f65:4a29;2a02:26f0:c900:b::5f65:4a31;2a02:26f0:c900:b::5f65:4a36</t>
+  </si>
+  <si>
+    <t>2.18.244.95; 2.18.244.99</t>
+  </si>
+  <si>
+    <t>Home Domain</t>
+  </si>
+  <si>
+    <t>www.defriesland.nl</t>
+  </si>
+  <si>
+    <t>www.fbto.nl</t>
+  </si>
+  <si>
+    <t>www.interpolis.nl</t>
+  </si>
+  <si>
+    <t>www.dechristelijkezorgverzekeraar.nl</t>
+  </si>
+  <si>
+    <t>www.zilverenkruis.nl</t>
+  </si>
+  <si>
+    <t>www.asr.nl</t>
+  </si>
+  <si>
+    <t>www.cz.nl</t>
+  </si>
+  <si>
+    <t>www.czdirect.cz.nl</t>
+  </si>
+  <si>
+    <t>www.nn.nl</t>
+  </si>
+  <si>
+    <t>www.just.nl</t>
+  </si>
+  <si>
+    <t>www.ohra.nl</t>
+  </si>
+  <si>
+    <t>www.dsw.nl</t>
+  </si>
+  <si>
+    <t>www.stadholland.nl</t>
+  </si>
+  <si>
+    <t>www.zorgenzekerheid.nl</t>
+  </si>
+  <si>
+    <t>www.unitedconsumers.com</t>
+  </si>
+  <si>
+    <t>www.salland.nl</t>
+  </si>
+  <si>
+    <t>www.anderzorg.nl</t>
+  </si>
+  <si>
+    <t>www.aevitae.com</t>
+  </si>
+  <si>
+    <t>www.menzis.nl</t>
+  </si>
+  <si>
+    <t>www.vgz.nl</t>
+  </si>
+  <si>
+    <t>www.vgzbewuzt.nl</t>
+  </si>
+  <si>
+    <t>www.zekur.nl</t>
+  </si>
+  <si>
+    <t>www.unive.nl</t>
+  </si>
+  <si>
+    <t>www.onvz.nl</t>
+  </si>
+  <si>
+    <t>www.vinkvink.nl</t>
+  </si>
+  <si>
+    <t>www.vvaa.nl</t>
+  </si>
+  <si>
+    <t>www.scheepvaartnet.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scheepvaartnet.nl/azvz-zorgverzekering/ </t>
+  </si>
+  <si>
+    <t>Login domain</t>
+  </si>
+  <si>
+    <t>Registration domain</t>
+  </si>
+  <si>
+    <t>www.bankieren.rabobank.nl</t>
+  </si>
+  <si>
+    <t>www.aanmelden.dsw.nl</t>
+  </si>
+  <si>
+    <t>www.aanmelden.stadholland.nl</t>
+  </si>
+  <si>
+    <t>www.aanvragen.aevitae.com</t>
+  </si>
+  <si>
+    <t>www.aanvraag.salland.nl</t>
+  </si>
+  <si>
+    <t>www.aanvragen.onvz.nl</t>
+  </si>
+  <si>
+    <t>www.aanvragen.vvaa.nl</t>
+  </si>
+  <si>
+    <t>www.service.zorgenzekerheid.nl</t>
+  </si>
+  <si>
+    <t>https://www.scheepvaartnet.nl/azvz-zorgverzekering/aanvraagformulier-azvz/</t>
+  </si>
+  <si>
+    <t>https://www.service.zorgenzekerheid.nl/advies/uwnawgegevens.html</t>
+  </si>
+  <si>
+    <t>www.login-select.fbto.nl</t>
+  </si>
+  <si>
+    <t>www.login-select.interpolis.nl</t>
+  </si>
+  <si>
+    <t>www.login-select.dechristelijkezorgverzekeraar.nl</t>
+  </si>
+  <si>
+    <t>www.login-select.zilverenkruis.nl</t>
+  </si>
+  <si>
+    <t>www.authenticatie.mijnzorg.asr.nl</t>
+  </si>
+  <si>
+    <t>www.authenticatie.mijnzorg-ikkieszelf.asr.nl</t>
+  </si>
+  <si>
+    <t>www.login.cz.nl</t>
+  </si>
+  <si>
+    <t>www.login.just.nl</t>
+  </si>
+  <si>
+    <t>www.login.nn-zorg.nl</t>
+  </si>
+  <si>
+    <t>www.login.ohra-zorg.nl</t>
+  </si>
+  <si>
+    <t>www.authenticatie.dsw.nl</t>
+  </si>
+  <si>
+    <t>www.authenticatie.stadholland.nl</t>
+  </si>
+  <si>
+    <t>www.mijn.salland.nl</t>
+  </si>
+  <si>
+    <t>www.idin.aevitae.com</t>
+  </si>
+  <si>
+    <t>www.inlog.anderzorg.nl</t>
+  </si>
+  <si>
+    <t>www.inlog.menzis.nl</t>
+  </si>
+  <si>
+    <t>www.inlog.vinkvink.nl</t>
+  </si>
+  <si>
+    <t>www.inlog.onvz.nl</t>
+  </si>
+  <si>
+    <t>www.prdledenvvaa.b2clogin.com</t>
+  </si>
+  <si>
+    <t>www.inloggen.mijnunivezorg.nl</t>
+  </si>
+  <si>
+    <t>www.inloggen.vgz.nl</t>
+  </si>
+  <si>
+    <t>www.inloggen.vgzbewuzt.nl</t>
+  </si>
+  <si>
+    <t>www.inloggen.mijnzekurzorg.nl</t>
+  </si>
+  <si>
     <t>login-select.defriesland.nl</t>
-  </si>
-  <si>
-    <t>login-select.interpolis.nl</t>
-  </si>
-  <si>
-    <t>login-select.dechristelijkezorgverzekeraar.nl</t>
-  </si>
-  <si>
-    <t>13.248.206.174;76.223.71.132</t>
-  </si>
-  <si>
-    <t>2600:9000:a61c:a0a1:422:c6a5:8963:492c;2600:9000:a50f:9f2b:9243:9933:1f8c:a16c</t>
-  </si>
-  <si>
-    <t>Check mijnzorg.fbto.nl where client see informations</t>
-  </si>
-  <si>
-    <t>login-select.fbto.nl</t>
-  </si>
-  <si>
-    <t>login-select.zilverenkruis.nl</t>
-  </si>
-  <si>
-    <t>authenticatie.mijnzorg.asr.nl</t>
-  </si>
-  <si>
-    <t>authenticatie.mijnzorg-ikkieszelf.asr.nl</t>
-  </si>
-  <si>
-    <t>2a02:26f0:c900:b::5f65:4a0c;2a02:26f0:c900:b::5f65:4a2c</t>
-  </si>
-  <si>
-    <t>2.18.244.78;2.18.244.78</t>
-  </si>
-  <si>
-    <t>login.cz.nl</t>
-  </si>
-  <si>
-    <t>login.just.nl</t>
-  </si>
-  <si>
-    <t>104.16.146.28;104.16.147.28</t>
-  </si>
-  <si>
-    <t>2606:4700::6810:921c;2606:4700::6810:931c</t>
-  </si>
-  <si>
-    <t>login.nn-zorg.nl</t>
-  </si>
-  <si>
-    <t>login.ohra-zorg.nl</t>
-  </si>
-  <si>
-    <t>Login ISP</t>
-  </si>
-  <si>
-    <t>Login cloud</t>
-  </si>
-  <si>
-    <t>authenticatie.dsw.nl</t>
-  </si>
-  <si>
-    <t>2a02:26f0:c900:b::5f65:4a13;2a02:26f0:c900:b::5f65:4a32</t>
-  </si>
-  <si>
-    <t>authenticatie.stadholland.nl</t>
-  </si>
-  <si>
-    <t>185.53.178.50</t>
-  </si>
-  <si>
-    <t>mijn.salland.nl</t>
-  </si>
-  <si>
-    <t>Support iDIN</t>
-  </si>
-  <si>
-    <t>inlog.anderzorg.nl</t>
-  </si>
-  <si>
-    <t>inlog.menzis.nl</t>
-  </si>
-  <si>
-    <t>inlog.vinkvink.nl</t>
-  </si>
-  <si>
-    <t>inlog.onvz.nl</t>
-  </si>
-  <si>
-    <t>prdledenvvaa.b2clogin.com</t>
-  </si>
-  <si>
-    <t>2603:1026:3000:148::7;2603:1026:3000:148::10;2603:1026:3000:150::a;2603:1026:3000:148::e;2603:1026:3000:150::5;2603:1026:3000:150::6;2603:1027:1:158::8;2603:1026:3000:150::8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
-    <t>20.190.160.17;20.190.160.22;40.126.32.76;40.126.32.136;20.190.160.14;40.126.32.140;40.126.32.68;40.126.32.74</t>
-  </si>
-  <si>
-    <t>idin.aevitae.com</t>
-  </si>
-  <si>
-    <t>109.68.90.49</t>
-  </si>
-  <si>
-    <t>inloggen.mijnunivezorg.nl</t>
-  </si>
-  <si>
-    <t>inloggen.mijnzekurzorg.nl</t>
-  </si>
-  <si>
-    <t>141.193.179.212</t>
-  </si>
-  <si>
-    <t>141.193.179.165</t>
-  </si>
-  <si>
-    <t>inloggen.vgz.nl</t>
-  </si>
-  <si>
-    <t>inloggen.vgzbewuzt.nl</t>
-  </si>
-  <si>
-    <t>Support login</t>
-  </si>
-  <si>
-    <t>64.113.50.231</t>
-  </si>
-  <si>
-    <t>141.193.179.238</t>
-  </si>
-  <si>
-    <t>Troy</t>
-  </si>
-  <si>
-    <t>ManagedWay</t>
-  </si>
-  <si>
-    <t>KPN</t>
-  </si>
-  <si>
-    <t>AS53292 ManagedWay;ManagedWay (managedway.com);ManagedWay;MWAY</t>
-  </si>
-  <si>
-    <t>ManagedWay;MWAY</t>
-  </si>
-  <si>
-    <t>MWAY</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microsoft </t>
-  </si>
-  <si>
-    <t>Microsoft Corporation</t>
-  </si>
-  <si>
-    <t>AS8075 Microsoft Corporation;Microsoft Corporation;Microsoft Corporation (microsoft.com)</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>ISP</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Amazon.com Inc.;Amazon.com, Inc.;AMAZON-02</t>
-  </si>
-  <si>
-    <t>AS16509 Amazon.com, Inc.;Amazon.com, Inc. (aws.com);AMAZON-02</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>CloudFlare</t>
-  </si>
-  <si>
-    <t>Cloudflare</t>
-  </si>
-  <si>
-    <t>AS13335 Cloudflare, Inc.;Cloudflare, Inc.;CLOUDFLARENET</t>
-  </si>
-  <si>
-    <t>CloudFlare Inc.;CLOUDFLARENET;Cloudflare</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Oslo</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>AS25148 ORANGE BUSINESS DIGITAL NORWAY AS;Signicat Vips</t>
-  </si>
-  <si>
-    <t>Orange Business Digital Norway AS;ORANGE BUSINESS DIGITAL NORWAY AS;Orange Business NO Network;ORANGE BUSINESS DIGITAL NORWAY AS;Basefarm Webdeal network</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Login Europa</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Munich</t>
-  </si>
-  <si>
-    <t>Akamai Technologies Inc.; Akamai International B.V.</t>
-  </si>
-  <si>
-    <t>AS20940 Akamai International B.V.;Akamai Technologies, Inc.;Akamai Technologies, Inc. (akamai.com);Akamai International B.V.</t>
-  </si>
-  <si>
-    <t>Akamai</t>
-  </si>
-  <si>
-    <t>San Jose</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>Home Location IP</t>
-  </si>
-  <si>
-    <t>Frankfurt</t>
-  </si>
-  <si>
-    <t>A100 ROW GmbH</t>
-  </si>
-  <si>
-    <t>A100 ROW GmbH;Amazon.com Inc.;Amazon.com, Inc.;AMAZON-02</t>
-  </si>
-  <si>
-    <t>Amazon germany</t>
-  </si>
-  <si>
-    <t>Amazone</t>
-  </si>
-  <si>
-    <t>Home in Europa</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Amsterdam</t>
-  </si>
-  <si>
-    <t>ASR Nederland N.V.;Asr Nederland N.V.;ASR Nederland N.V.</t>
-  </si>
-  <si>
-    <t>AS50737 ASR Nederland N.V.; Asr Nederland N.V. (asr.nl); ASR Nederland N.V.</t>
-  </si>
-  <si>
-    <t>Tilburg</t>
-  </si>
-  <si>
-    <t>AS1136 KPN B.V.;Cz Groep Zorgverzekeringen (kpn.net);KPN B.V.</t>
-  </si>
-  <si>
-    <t>KPN CZ</t>
-  </si>
-  <si>
-    <t>KPN B.V.</t>
-  </si>
-  <si>
-    <t>AS16625 Akamai Technologies, Inc.</t>
-  </si>
-  <si>
-    <t>Akamai Amsterdam</t>
-  </si>
-  <si>
-    <t>Akamai Technologies, Inc.</t>
-  </si>
-  <si>
-    <t>AS9150 Interconnect;ML Consultancy;Indicia e-Business B.V.</t>
-  </si>
-  <si>
-    <t>Indicia e-Business B.V.; MLC/InterConnect; Ml Consultancy; MLC/InterConnect routed block</t>
-  </si>
-  <si>
-    <t>s-Hertogenbosch</t>
-  </si>
-  <si>
-    <t>Interconnect</t>
-  </si>
-  <si>
-    <t>interconnect</t>
-  </si>
-  <si>
-    <t>Claranet</t>
-  </si>
-  <si>
-    <t>AS8426 Claranet Limited;UnitedConsumers Brand &amp; IP B.V;Unitedconsumers Brand &amp; Ip B.V. (unitedconsumers.com)</t>
-  </si>
-  <si>
-    <t>UnitedConsumers Brand &amp; IP B.V.;Claranet Limited</t>
-  </si>
-  <si>
-    <t>Registration europa</t>
-  </si>
-  <si>
-    <t>Registration IPv4</t>
-  </si>
-  <si>
-    <t>193.173.52.131</t>
-  </si>
-  <si>
-    <t>Registration Location</t>
-  </si>
-  <si>
-    <t>Netherlandse</t>
-  </si>
-  <si>
-    <t>https://www.unitedconsumers.com/zorgverzekering/aanmelden/offerte.asp</t>
-  </si>
-  <si>
-    <t>https://www.zekur.nl/zorgverzekering/afsluiten</t>
-  </si>
-  <si>
-    <t>https://www.defriesland.nl/zorgverzekering/premie-berekenen/persoonsgegevens</t>
-  </si>
-  <si>
-    <t>https://www.fbto.nl/zorgverzekering/premie-berekenen/naam</t>
-  </si>
-  <si>
-    <t>https://bankieren.rabobank.nl/</t>
-  </si>
-  <si>
-    <t>https://www.dechristelijkezorgverzekeraar.nl/zorgverzekering/premie-berekenen/persoonsgegevens</t>
-  </si>
-  <si>
-    <t>https://www.zilverenkruis.nl/consumenten/zorgverzekering/premie-berekenen/persoonsgegevens</t>
-  </si>
-  <si>
-    <t>https://www.asr.nl/verzekeringen/zorgverzekering/afsluiten#/user-data</t>
-  </si>
-  <si>
-    <t>https://www.asr.nl/verzekeringen/zorgverzekering/ikkieszelf/afsluiten#/user-data</t>
-  </si>
-  <si>
-    <t>https://www.cz.nl/zorgverzekering/premie-berekenen/aanmelden</t>
-  </si>
-  <si>
-    <t>https://www.just.nl/zorgverzekering/premie-berekenen/aanmelden</t>
-  </si>
-  <si>
-    <t>https://www.czdirect.cz.nl/zorgverzekering/premie-berekenen/aanmelden</t>
-  </si>
-  <si>
-    <t>https://www.nn.nl/Particulier/Zorgverzekering/Zorgverzekering-aanvragen.htm#aanvrager</t>
-  </si>
-  <si>
-    <t>https://www.ohra.nl/zorgverzekering/berekenen#aanvrager</t>
-  </si>
-  <si>
-    <t>https://aanmelden.dsw.nl/aanmelden</t>
-  </si>
-  <si>
-    <t>https://aanmelden.stadholland.nl/</t>
-  </si>
-  <si>
-    <t>Registration traditioneel</t>
-  </si>
-  <si>
-    <t>https://aanvraag.salland.nl/persoonsgegevens</t>
-  </si>
-  <si>
-    <t>https://aanvragen.aevitae.com/nl/44086/personal_data</t>
-  </si>
-  <si>
-    <t>https://www.anderzorg.nl/premie-berekenen-en-aanvragen</t>
-  </si>
-  <si>
-    <t>https://www.menzis.nl/premie-berekenen-en-aanvragen</t>
-  </si>
-  <si>
-    <t>https://www.vinkvink.nl/premie-berekenen-en-aanvragen</t>
-  </si>
-  <si>
-    <t>https://aanvragen.onvz.nl/index.html</t>
-  </si>
-  <si>
-    <t>https://aanvragen.vvaazorgverzekering.nl/index.html</t>
-  </si>
-  <si>
-    <t>https://www.vgzbewuzt.nl/premie-berekenen/stap4</t>
-  </si>
-  <si>
-    <t>https://www.vgz.nl/zorgverzekering/premie-berekenen-en-afsluiten#/stap2</t>
-  </si>
-  <si>
-    <t>https://www.unive.nl/verzekeringspakket/premieberekenen-en-afsluiten/Gegevens?AanvraagId=54542</t>
-  </si>
-  <si>
-    <t>Registration vs Home</t>
-  </si>
-  <si>
-    <t>Login vs Home</t>
-  </si>
-  <si>
-    <t>13.107.246.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2620:1ec:bdf::67</t>
-  </si>
-  <si>
-    <t>141.101.90.104;141.101.90.105;141.101.90.106;141.101.90.107</t>
-  </si>
-  <si>
-    <t>2a06:98c1:3200::90:80;2a06:98c1:3200::90:81;2a06:98c1:3200::90:82;2a06:98c1:3200::90:83</t>
-  </si>
-  <si>
-    <t>2a05:d014:145:aa02:39cc:ca87:679c:1a44;2a05:d014:145:aa01:e7ed:1bdf:317c:168e;2a05:d014:145:aa00:63e4:ad8e:c1c7:8675</t>
-  </si>
-  <si>
-    <t>3.125.189.196;3.126.216.110;3.127.11.115</t>
-  </si>
-  <si>
-    <t>2a02:26f0:c900:b::5f65:4a23;2a02:26f0:c900:b::5f65:4a27;2a02:26f0:c900:b::5f65:4a29;2a02:26f0:c900:b::5f65:4a31;2a02:26f0:c900:b::5f65:4a36</t>
-  </si>
-  <si>
-    <t>2.18.244.95; 2.18.244.99</t>
-  </si>
-  <si>
-    <t>Home Domain</t>
-  </si>
-  <si>
-    <t>www.defriesland.nl</t>
-  </si>
-  <si>
-    <t>www.fbto.nl</t>
-  </si>
-  <si>
-    <t>www.interpolis.nl</t>
-  </si>
-  <si>
-    <t>www.dechristelijkezorgverzekeraar.nl</t>
-  </si>
-  <si>
-    <t>www.zilverenkruis.nl</t>
-  </si>
-  <si>
-    <t>www.asr.nl</t>
-  </si>
-  <si>
-    <t>www.cz.nl</t>
-  </si>
-  <si>
-    <t>www.czdirect.cz.nl</t>
-  </si>
-  <si>
-    <t>www.nn.nl</t>
-  </si>
-  <si>
-    <t>www.just.nl</t>
-  </si>
-  <si>
-    <t>www.ohra.nl</t>
-  </si>
-  <si>
-    <t>www.dsw.nl</t>
-  </si>
-  <si>
-    <t>www.stadholland.nl</t>
-  </si>
-  <si>
-    <t>www.zorgenzekerheid.nl</t>
-  </si>
-  <si>
-    <t>www.unitedconsumers.com</t>
-  </si>
-  <si>
-    <t>www.salland.nl</t>
-  </si>
-  <si>
-    <t>www.anderzorg.nl</t>
-  </si>
-  <si>
-    <t>www.aevitae.com</t>
-  </si>
-  <si>
-    <t>www.menzis.nl</t>
-  </si>
-  <si>
-    <t>www.vgz.nl</t>
-  </si>
-  <si>
-    <t>www.vgzbewuzt.nl</t>
-  </si>
-  <si>
-    <t>www.zekur.nl</t>
-  </si>
-  <si>
-    <t>www.unive.nl</t>
-  </si>
-  <si>
-    <t>www.onvz.nl</t>
-  </si>
-  <si>
-    <t>www.vinkvink.nl</t>
-  </si>
-  <si>
-    <t>www.vvaa.nl</t>
-  </si>
-  <si>
-    <t>www.scheepvaartnet.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.scheepvaartnet.nl/azvz-zorgverzekering/ </t>
-  </si>
-  <si>
-    <t>Login domain</t>
-  </si>
-  <si>
-    <t>Registration domain</t>
-  </si>
-  <si>
-    <t>www.bankieren.rabobank.nl</t>
-  </si>
-  <si>
-    <t>www.aanmelden.dsw.nl</t>
-  </si>
-  <si>
-    <t>www.aanmelden.stadholland.nl</t>
-  </si>
-  <si>
-    <t>www.aanvragen.aevitae.com</t>
-  </si>
-  <si>
-    <t>www.aanvraag.salland.nl</t>
-  </si>
-  <si>
-    <t>www.aanvragen.onvz.nl</t>
-  </si>
-  <si>
-    <t>www.aanvragen.vvaa.nl</t>
-  </si>
-  <si>
-    <t>www.service.zorgenzekerheid.nl</t>
-  </si>
-  <si>
-    <t>https://www.scheepvaartnet.nl/azvz-zorgverzekering/aanvraagformulier-azvz/</t>
-  </si>
-  <si>
-    <t>https://www.service.zorgenzekerheid.nl/advies/uwnawgegevens.html</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2133,7 @@
   <dimension ref="A1:BT29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AZ6" sqref="AZ6:AZ29"/>
+      <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,10 +2215,10 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="F1" t="s">
         <v>148</v>
@@ -2230,7 +2230,7 @@
         <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="J1" t="s">
         <v>262</v>
@@ -2239,7 +2239,7 @@
         <v>169</v>
       </c>
       <c r="L1" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="M1" t="s">
         <v>183</v>
@@ -2278,7 +2278,7 @@
         <v>160</v>
       </c>
       <c r="Y1" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="Z1" t="s">
         <v>135</v>
@@ -2290,25 +2290,25 @@
         <v>137</v>
       </c>
       <c r="AC1" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="AD1" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="AE1" t="s">
         <v>133</v>
       </c>
       <c r="AF1" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="AG1" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="AH1" t="s">
         <v>161</v>
       </c>
       <c r="AI1" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="AJ1" t="s">
         <v>185</v>
@@ -2347,7 +2347,7 @@
         <v>168</v>
       </c>
       <c r="AV1" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="AW1" t="s">
         <v>139</v>
@@ -2359,10 +2359,10 @@
         <v>141</v>
       </c>
       <c r="AZ1" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="BA1" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="BB1" t="s">
         <v>266</v>
@@ -2374,10 +2374,10 @@
         <v>142</v>
       </c>
       <c r="BE1" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="BF1" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="BG1" t="s">
         <v>201</v>
@@ -2410,7 +2410,7 @@
         <v>143</v>
       </c>
       <c r="BQ1" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="BR1" t="s">
         <v>157</v>
@@ -2448,7 +2448,7 @@
         <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="J2" t="s">
         <v>242</v>
@@ -2457,13 +2457,13 @@
         <v>243</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -2514,10 +2514,10 @@
         <v>1</v>
       </c>
       <c r="AE2" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="AF2" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="AG2" t="s">
         <v>242</v>
@@ -2526,13 +2526,13 @@
         <v>243</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL2">
         <v>1</v>
@@ -2579,29 +2579,29 @@
       <c r="AZ2">
         <v>0</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BA2" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="BB2" t="s">
         <v>269</v>
       </c>
-      <c r="BB2" t="s">
-        <v>272</v>
-      </c>
       <c r="BC2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BD2" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="BE2" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BF2" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BG2">
         <v>1</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI2">
         <v>1</v>
@@ -2666,7 +2666,7 @@
         <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="J3" t="s">
         <v>242</v>
@@ -2675,13 +2675,13 @@
         <v>243</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M3" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N3" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -2732,10 +2732,10 @@
         <v>1</v>
       </c>
       <c r="AE3" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="AF3" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="AG3" t="s">
         <v>242</v>
@@ -2744,13 +2744,13 @@
         <v>243</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ3" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK3" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL3">
         <v>1</v>
@@ -2797,29 +2797,29 @@
       <c r="AZ3">
         <v>0</v>
       </c>
-      <c r="BA3" t="s">
-        <v>275</v>
+      <c r="BA3" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="BB3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BC3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BD3" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="BE3" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BF3" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BG3">
         <v>1</v>
       </c>
       <c r="BH3" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI3">
         <v>1</v>
@@ -2884,7 +2884,7 @@
         <v>73</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="J4" t="s">
         <v>242</v>
@@ -2893,13 +2893,13 @@
         <v>243</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M4" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N4" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -2950,25 +2950,25 @@
         <v>0</v>
       </c>
       <c r="AE4" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="AF4" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
       <c r="AG4" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="AH4" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="AI4" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="AJ4" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL4">
         <v>1</v>
@@ -3015,29 +3015,29 @@
       <c r="AZ4">
         <v>0</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BA4" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>269</v>
+      </c>
+      <c r="BC4" t="s">
         <v>270</v>
       </c>
-      <c r="BB4" t="s">
-        <v>272</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>273</v>
-      </c>
       <c r="BD4" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="BE4" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BF4" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BG4">
         <v>1</v>
       </c>
       <c r="BH4" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI4">
         <v>1</v>
@@ -3102,7 +3102,7 @@
         <v>77</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="J5" t="s">
         <v>242</v>
@@ -3111,13 +3111,13 @@
         <v>243</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M5" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N5" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -3168,10 +3168,10 @@
         <v>1</v>
       </c>
       <c r="AE5" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="AF5" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="AG5" t="s">
         <v>242</v>
@@ -3180,13 +3180,13 @@
         <v>243</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ5" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK5" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL5">
         <v>1</v>
@@ -3233,29 +3233,29 @@
       <c r="AZ5">
         <v>0</v>
       </c>
-      <c r="BA5" t="s">
-        <v>271</v>
+      <c r="BA5" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="BB5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BC5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BD5" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="BE5" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BF5" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BG5">
         <v>1</v>
       </c>
       <c r="BH5" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI5">
         <v>1</v>
@@ -3320,7 +3320,7 @@
         <v>78</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="J6" t="s">
         <v>242</v>
@@ -3329,13 +3329,13 @@
         <v>243</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M6" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N6" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -3386,10 +3386,10 @@
         <v>1</v>
       </c>
       <c r="AE6" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="AF6" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="AG6" t="s">
         <v>242</v>
@@ -3398,13 +3398,13 @@
         <v>243</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ6" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK6" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL6">
         <v>1</v>
@@ -3451,29 +3451,29 @@
       <c r="AZ6">
         <v>0</v>
       </c>
-      <c r="BA6" t="s">
-        <v>276</v>
+      <c r="BA6" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="BB6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BC6" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BD6" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="BE6" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BF6" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BG6">
         <v>1</v>
       </c>
       <c r="BH6" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI6">
         <v>1</v>
@@ -3538,13 +3538,13 @@
         <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J7" t="s">
         <v>244</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M7" t="s">
         <v>9</v>
@@ -3601,16 +3601,16 @@
         <v>1</v>
       </c>
       <c r="AE7" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="AF7" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="AG7" t="s">
         <v>244</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ7" t="s">
         <v>9</v>
@@ -3663,23 +3663,23 @@
       <c r="AZ7">
         <v>0</v>
       </c>
-      <c r="BA7" t="s">
-        <v>277</v>
+      <c r="BA7" s="1" t="s">
+        <v>439</v>
       </c>
       <c r="BB7" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="BC7" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="BD7" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="BE7" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BF7" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BG7">
         <v>1</v>
@@ -3750,13 +3750,13 @@
         <v>84</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J8" t="s">
         <v>244</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M8" t="s">
         <v>9</v>
@@ -3813,16 +3813,16 @@
         <v>1</v>
       </c>
       <c r="AE8" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="AF8" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="AG8" t="s">
         <v>244</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ8" t="s">
         <v>9</v>
@@ -3875,23 +3875,23 @@
       <c r="AZ8">
         <v>0</v>
       </c>
-      <c r="BA8" t="s">
-        <v>278</v>
+      <c r="BA8" s="1" t="s">
+        <v>440</v>
       </c>
       <c r="BB8" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="BC8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="BD8" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="BE8" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BF8" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BG8">
         <v>1</v>
@@ -3962,19 +3962,19 @@
         <v>85</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="J9" t="s">
         <v>245</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="M9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -4025,22 +4025,22 @@
         <v>1</v>
       </c>
       <c r="AE9" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="AF9" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="AG9" t="s">
         <v>245</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="AJ9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL9">
         <v>1</v>
@@ -4087,29 +4087,29 @@
       <c r="AZ9">
         <v>0</v>
       </c>
-      <c r="BA9" t="s">
-        <v>281</v>
+      <c r="BA9" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="BB9" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC9" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD9" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="BE9" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF9" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG9">
         <v>1</v>
       </c>
       <c r="BH9" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI9">
         <v>1</v>
@@ -4174,19 +4174,19 @@
         <v>247</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>246</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M10" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N10" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O10">
         <v>1</v>
@@ -4237,22 +4237,22 @@
         <v>1</v>
       </c>
       <c r="AE10" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="AF10" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>246</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ10" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK10" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL10">
         <v>1</v>
@@ -4299,29 +4299,29 @@
       <c r="AZ10">
         <v>0</v>
       </c>
-      <c r="BA10" t="s">
-        <v>281</v>
+      <c r="BA10" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="BB10" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC10" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD10" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="BE10" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF10" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG10">
         <v>1</v>
       </c>
       <c r="BH10" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI10">
         <v>1</v>
@@ -4386,25 +4386,25 @@
         <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>245</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="M11" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N11" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -4449,28 +4449,28 @@
         <v>1</v>
       </c>
       <c r="AE11" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="AF11" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>245</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="AJ11" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK11" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL11">
         <v>1</v>
       </c>
       <c r="AM11" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="AN11">
         <v>0</v>
@@ -4511,29 +4511,29 @@
       <c r="AZ11">
         <v>0</v>
       </c>
-      <c r="BA11" t="s">
-        <v>282</v>
+      <c r="BA11" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="BB11" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC11" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD11" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="BE11" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF11" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG11">
         <v>1</v>
       </c>
       <c r="BH11" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI11">
         <v>1</v>
@@ -4598,7 +4598,7 @@
         <v>89</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>253</v>
@@ -4607,13 +4607,13 @@
         <v>249</v>
       </c>
       <c r="L12" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="M12" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -4664,10 +4664,10 @@
         <v>1</v>
       </c>
       <c r="AE12" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="AF12" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>253</v>
@@ -4676,13 +4676,13 @@
         <v>249</v>
       </c>
       <c r="AI12" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="AJ12" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL12">
         <v>1</v>
@@ -4729,29 +4729,29 @@
       <c r="AZ12">
         <v>0</v>
       </c>
-      <c r="BA12" t="s">
-        <v>285</v>
+      <c r="BA12" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="BB12" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC12" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD12" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="BE12" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF12" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG12">
         <v>1</v>
       </c>
       <c r="BH12" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI12">
         <v>1</v>
@@ -4816,7 +4816,7 @@
         <v>74</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>250</v>
@@ -4825,13 +4825,13 @@
         <v>251</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="M13" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -4882,10 +4882,10 @@
         <v>1</v>
       </c>
       <c r="AE13" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="AF13" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>250</v>
@@ -4894,13 +4894,13 @@
         <v>251</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="AJ13" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL13">
         <v>1</v>
@@ -4947,29 +4947,29 @@
       <c r="AZ13">
         <v>0</v>
       </c>
-      <c r="BA13" t="s">
-        <v>286</v>
+      <c r="BA13" s="1" t="s">
+        <v>444</v>
       </c>
       <c r="BB13" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC13" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD13" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="BE13" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF13" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG13">
         <v>1</v>
       </c>
       <c r="BH13" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI13">
         <v>1</v>
@@ -5034,22 +5034,22 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>252</v>
       </c>
       <c r="K14" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M14" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -5100,25 +5100,25 @@
         <v>0</v>
       </c>
       <c r="AE14" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="AF14" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="AG14" s="1" t="s">
         <v>252</v>
       </c>
       <c r="AH14" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ14" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL14">
         <v>1</v>
@@ -5165,29 +5165,29 @@
       <c r="AZ14">
         <v>0</v>
       </c>
-      <c r="BA14" t="s">
-        <v>289</v>
+      <c r="BA14" s="1" t="s">
+        <v>445</v>
       </c>
       <c r="BB14" t="s">
         <v>252</v>
       </c>
       <c r="BC14" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="BD14" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="BE14" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BF14" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BG14">
         <v>1</v>
       </c>
       <c r="BH14" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI14">
         <v>1</v>
@@ -5252,22 +5252,22 @@
         <v>91</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>252</v>
       </c>
       <c r="K15" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M15" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -5318,25 +5318,25 @@
         <v>0</v>
       </c>
       <c r="AE15" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="AF15" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="AG15" s="1" t="s">
         <v>252</v>
       </c>
       <c r="AH15" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ15" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK15" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL15">
         <v>1</v>
@@ -5383,29 +5383,29 @@
       <c r="AZ15">
         <v>0</v>
       </c>
-      <c r="BA15" t="s">
-        <v>291</v>
+      <c r="BA15" s="1" t="s">
+        <v>446</v>
       </c>
       <c r="BB15" t="s">
         <v>252</v>
       </c>
       <c r="BC15" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="BD15" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="BE15" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BF15" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="BG15">
         <v>1</v>
       </c>
       <c r="BH15" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI15">
         <v>1</v>
@@ -5470,19 +5470,19 @@
         <v>90</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>254</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M16" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O16">
         <v>1</v>
@@ -5533,25 +5533,25 @@
         <v>0</v>
       </c>
       <c r="AE16" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="AF16" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="AH16" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="AJ16" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AL16">
         <v>1</v>
@@ -5598,26 +5598,29 @@
       <c r="AZ16">
         <v>0</v>
       </c>
-      <c r="BA16" t="s">
-        <v>293</v>
+      <c r="BA16" s="1" t="s">
+        <v>447</v>
       </c>
       <c r="BB16" t="s">
-        <v>292</v>
+        <v>388</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>389</v>
       </c>
       <c r="BD16" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="BE16" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF16" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG16">
         <v>1</v>
       </c>
       <c r="BH16" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="BI16">
         <v>1</v>
@@ -5682,7 +5685,7 @@
         <v>92</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>256</v>
@@ -5691,19 +5694,19 @@
         <v>255</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="M17" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="Q17">
         <v>1</v>
@@ -5748,25 +5751,25 @@
         <v>0</v>
       </c>
       <c r="AE17" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="AF17" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
       <c r="AG17" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="AH17" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="AJ17" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK17" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL17">
         <v>1</v>
@@ -5813,26 +5816,26 @@
       <c r="AZ17">
         <v>0</v>
       </c>
-      <c r="BA17" t="s">
-        <v>303</v>
+      <c r="BA17" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="BB17" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="BD17" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="BE17" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="BF17" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="BG17">
         <v>1</v>
       </c>
       <c r="BH17" s="1" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="BI17">
         <v>0</v>
@@ -5897,19 +5900,19 @@
         <v>93</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>259</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M18" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O18">
         <v>1</v>
@@ -5960,22 +5963,22 @@
         <v>1</v>
       </c>
       <c r="AE18" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="AF18" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="AG18" s="1" t="s">
         <v>259</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ18" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL18">
         <v>1</v>
@@ -6022,29 +6025,29 @@
       <c r="AZ18">
         <v>0</v>
       </c>
-      <c r="BA18" t="s">
-        <v>295</v>
+      <c r="BA18" s="1" t="s">
+        <v>449</v>
       </c>
       <c r="BB18" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC18" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD18" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="BE18" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF18" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG18">
         <v>1</v>
       </c>
       <c r="BH18" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI18">
         <v>1</v>
@@ -6109,19 +6112,19 @@
         <v>66</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>259</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M19" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -6172,22 +6175,22 @@
         <v>1</v>
       </c>
       <c r="AE19" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="AF19" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="AG19" s="1" t="s">
         <v>259</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ19" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK19" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL19">
         <v>1</v>
@@ -6234,29 +6237,29 @@
       <c r="AZ19">
         <v>0</v>
       </c>
-      <c r="BA19" t="s">
+      <c r="BA19" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>274</v>
+      </c>
+      <c r="BC19" t="s">
+        <v>275</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>325</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>309</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>309</v>
+      </c>
+      <c r="BG19">
+        <v>1</v>
+      </c>
+      <c r="BH19" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="BB19" t="s">
-        <v>283</v>
-      </c>
-      <c r="BC19" t="s">
-        <v>284</v>
-      </c>
-      <c r="BD19" t="s">
-        <v>349</v>
-      </c>
-      <c r="BE19" t="s">
-        <v>333</v>
-      </c>
-      <c r="BF19" t="s">
-        <v>333</v>
-      </c>
-      <c r="BG19">
-        <v>1</v>
-      </c>
-      <c r="BH19" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="BI19">
         <v>1</v>
@@ -6321,19 +6324,19 @@
         <v>67</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>259</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M20" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -6384,22 +6387,22 @@
         <v>1</v>
       </c>
       <c r="AE20" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="AF20" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="AG20" s="1" t="s">
         <v>259</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ20" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK20" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL20">
         <v>1</v>
@@ -6446,29 +6449,29 @@
       <c r="AZ20">
         <v>0</v>
       </c>
-      <c r="BA20" t="s">
-        <v>297</v>
+      <c r="BA20" s="1" t="s">
+        <v>451</v>
       </c>
       <c r="BB20" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BC20" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="BD20" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="BE20" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BF20" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="BG20">
         <v>1</v>
       </c>
       <c r="BH20" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI20">
         <v>1</v>
@@ -6533,7 +6536,7 @@
         <v>94</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>260</v>
@@ -6542,19 +6545,19 @@
         <v>261</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="M21" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="O21">
         <v>1</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="Q21">
         <v>1</v>
@@ -6599,31 +6602,31 @@
         <v>0</v>
       </c>
       <c r="AE21" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AF21" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="AG21" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="AH21" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="AJ21" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="AK21" s="1" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="AL21">
         <v>1</v>
       </c>
       <c r="AM21" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="AN21">
         <v>1</v>
@@ -6664,29 +6667,29 @@
       <c r="AZ21">
         <v>0</v>
       </c>
-      <c r="BA21" t="s">
-        <v>298</v>
+      <c r="BA21" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="BB21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BC21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BD21" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="BE21" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BF21" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BG21">
         <v>1</v>
       </c>
       <c r="BH21" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI21">
         <v>1</v>
@@ -6751,7 +6754,7 @@
         <v>83</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>256</v>
@@ -6760,19 +6763,19 @@
         <v>255</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="M22" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O22">
         <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="Q22">
         <v>1</v>
@@ -6817,31 +6820,31 @@
         <v>0</v>
       </c>
       <c r="AE22" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="AF22" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
       <c r="AG22" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="AH22" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="AJ22" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="AL22">
         <v>1</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="AN22">
         <v>1</v>
@@ -6882,23 +6885,23 @@
       <c r="AZ22">
         <v>0</v>
       </c>
-      <c r="BA22" t="s">
-        <v>299</v>
+      <c r="BA22" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="BB22" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="BC22" t="s">
+        <v>280</v>
+      </c>
+      <c r="BD22" t="s">
         <v>300</v>
       </c>
-      <c r="BD22" t="s">
-        <v>324</v>
-      </c>
       <c r="BE22" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="BF22" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="BG22">
         <v>1</v>
@@ -6969,19 +6972,19 @@
         <v>88</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>263</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M23" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O23">
         <v>1</v>
@@ -7032,25 +7035,25 @@
         <v>1</v>
       </c>
       <c r="AE23" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="AF23" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
       <c r="AG23" s="1" t="s">
         <v>263</v>
       </c>
       <c r="AH23" t="s">
+        <v>281</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AJ23" t="s">
         <v>301</v>
       </c>
-      <c r="AI23" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>325</v>
-      </c>
       <c r="AK23" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL23">
         <v>1</v>
@@ -7097,26 +7100,26 @@
       <c r="AZ23">
         <v>0</v>
       </c>
-      <c r="BA23" t="s">
-        <v>305</v>
+      <c r="BA23" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="BB23" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="BD23" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="BE23" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BF23" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BG23">
         <v>1</v>
       </c>
       <c r="BH23" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI23">
         <v>0</v>
@@ -7181,19 +7184,19 @@
         <v>82</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>264</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M24" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N24" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -7244,22 +7247,22 @@
         <v>1</v>
       </c>
       <c r="AE24" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="AF24" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>264</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ24" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK24" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL24">
         <v>1</v>
@@ -7306,26 +7309,26 @@
       <c r="AZ24">
         <v>0</v>
       </c>
-      <c r="BA24" t="s">
-        <v>309</v>
+      <c r="BA24" s="1" t="s">
+        <v>455</v>
       </c>
       <c r="BB24" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="BD24" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="BE24" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BF24" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BG24">
         <v>1</v>
       </c>
       <c r="BH24" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI24">
         <v>0</v>
@@ -7390,19 +7393,19 @@
         <v>68</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>264</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M25" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="N25" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="O25">
         <v>1</v>
@@ -7453,22 +7456,22 @@
         <v>1</v>
       </c>
       <c r="AE25" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="AF25" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="AG25" s="1" t="s">
         <v>264</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ25" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AK25" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="AL25">
         <v>1</v>
@@ -7515,26 +7518,26 @@
       <c r="AZ25">
         <v>0</v>
       </c>
-      <c r="BA25" t="s">
-        <v>310</v>
+      <c r="BA25" s="1" t="s">
+        <v>456</v>
       </c>
       <c r="BB25" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="BD25" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="BE25" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BF25" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BG25">
         <v>1</v>
       </c>
       <c r="BH25" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI25">
         <v>0</v>
@@ -7599,19 +7602,19 @@
         <v>75</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="J26" t="s">
         <v>241</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="M26" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="O26">
         <v>1</v>
@@ -7662,22 +7665,22 @@
         <v>1</v>
       </c>
       <c r="AE26" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="AF26" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="AG26" t="s">
         <v>241</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="AJ26" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="AK26" s="1" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="AL26">
         <v>1</v>
@@ -7724,26 +7727,26 @@
       <c r="AZ26">
         <v>0</v>
       </c>
-      <c r="BA26" t="s">
-        <v>306</v>
+      <c r="BA26" s="1" t="s">
+        <v>457</v>
       </c>
       <c r="BB26" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="BD26" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="BE26" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BF26" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BG26">
         <v>1</v>
       </c>
       <c r="BH26" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI26">
         <v>0</v>
@@ -7808,19 +7811,19 @@
         <v>80</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="J27" t="s">
         <v>240</v>
       </c>
       <c r="L27" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="M27" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="O27">
         <v>1</v>
@@ -7871,22 +7874,22 @@
         <v>1</v>
       </c>
       <c r="AE27" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="AF27" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="AG27" t="s">
         <v>240</v>
       </c>
       <c r="AI27" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AJ27" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="AK27" s="1" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="AL27">
         <v>1</v>
@@ -7933,26 +7936,26 @@
       <c r="AZ27">
         <v>0</v>
       </c>
-      <c r="BA27" t="s">
-        <v>309</v>
+      <c r="BA27" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="BB27" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="BD27" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="BE27" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BF27" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="BG27">
         <v>1</v>
       </c>
       <c r="BH27" s="1" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="BI27">
         <v>0</v>
@@ -8014,10 +8017,10 @@
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="J28" t="s">
         <v>175</v>
@@ -8026,10 +8029,10 @@
         <v>177</v>
       </c>
       <c r="M28" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="N28" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="O28">
         <v>1</v>
@@ -8080,10 +8083,10 @@
         <v>1</v>
       </c>
       <c r="AE28" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
       <c r="AF28" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="AG28" t="s">
         <v>175</v>
@@ -8093,10 +8096,10 @@
         <v>177</v>
       </c>
       <c r="AJ28" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="AK28" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="AL28">
         <v>1</v>
@@ -8153,10 +8156,10 @@
         <v>182</v>
       </c>
       <c r="BE28" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="BF28" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="BG28">
         <v>1</v>
@@ -8227,7 +8230,7 @@
         <v>81</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>257</v>
@@ -8236,19 +8239,19 @@
         <v>258</v>
       </c>
       <c r="L29" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="M29" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="N29" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="O29">
         <v>1</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -8293,28 +8296,28 @@
         <v>0</v>
       </c>
       <c r="AE29" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="AF29" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="AG29" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="AI29" t="s">
         <v>182</v>
       </c>
       <c r="AJ29" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="AK29" s="1" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="AL29">
         <v>1</v>
       </c>
       <c r="AM29" s="1" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="AN29">
         <v>0</v>
@@ -8365,10 +8368,10 @@
         <v>182</v>
       </c>
       <c r="BE29" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="BF29" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="BG29">
         <v>1</v>
@@ -9333,6 +9336,32 @@
     <hyperlink ref="AF19" r:id="rId93" xr:uid="{70A5BAAA-5790-4919-8346-E017C3255984}"/>
     <hyperlink ref="AF14" r:id="rId94" xr:uid="{9129E375-E5C7-43F9-AB82-3C6F6638EBD4}"/>
     <hyperlink ref="AE29" r:id="rId95" xr:uid="{952A0304-5B2C-4D4B-BA4A-D4C03F0B7612}"/>
+    <hyperlink ref="BA2" r:id="rId96" display="www.login-select.defriesland.nl" xr:uid="{0DDE0281-20FA-4487-9DA2-33A55F53257D}"/>
+    <hyperlink ref="BA3" r:id="rId97" xr:uid="{036F04D4-28B1-4A93-AF12-F2496F10EE17}"/>
+    <hyperlink ref="BA4" r:id="rId98" xr:uid="{90E9A6A1-A3BB-4174-8382-22CFE2944455}"/>
+    <hyperlink ref="BA5" r:id="rId99" xr:uid="{7D7AD1B5-E971-43C8-8BCE-E0CEEFEF2C08}"/>
+    <hyperlink ref="BA6" r:id="rId100" xr:uid="{F6A59FE3-1075-431D-BEED-E05A288E1B1E}"/>
+    <hyperlink ref="BA7" r:id="rId101" xr:uid="{EACA0B4B-086C-425D-BF2A-2C9D9021EE71}"/>
+    <hyperlink ref="BA8" r:id="rId102" xr:uid="{22E99511-D9A2-4E9B-A92C-80D00A18043D}"/>
+    <hyperlink ref="BA9" r:id="rId103" xr:uid="{6C435B83-9690-4EAF-891D-1DC5CB0E91C8}"/>
+    <hyperlink ref="BA10" r:id="rId104" xr:uid="{D1A97DE9-BA5E-41DC-A0C2-0725799FCE1B}"/>
+    <hyperlink ref="BA11" r:id="rId105" xr:uid="{2078425F-9C83-4AA3-820D-3801DB190F75}"/>
+    <hyperlink ref="BA12" r:id="rId106" xr:uid="{3A491BF6-69EC-4639-A95D-71D1A0A6D5F5}"/>
+    <hyperlink ref="BA13" r:id="rId107" xr:uid="{F21DF260-3ADF-4FFC-89F8-6D57D34A7F9B}"/>
+    <hyperlink ref="BA14" r:id="rId108" xr:uid="{ECBB63B6-798A-4B39-AB6E-5B312E6A2E88}"/>
+    <hyperlink ref="BA15" r:id="rId109" xr:uid="{6733EE79-87A3-4E41-8BF5-2383B09DDB83}"/>
+    <hyperlink ref="BA16" r:id="rId110" xr:uid="{D5299527-4779-4E5C-9371-03A039584659}"/>
+    <hyperlink ref="BA17" r:id="rId111" xr:uid="{0DB09F74-398F-4AFE-87BB-9C06F7C4D3CE}"/>
+    <hyperlink ref="BA18" r:id="rId112" xr:uid="{C4CB4073-EA13-4845-BA77-E73A2C93C5A5}"/>
+    <hyperlink ref="BA19" r:id="rId113" xr:uid="{40549E75-A603-42DE-A106-3AFE97E9F915}"/>
+    <hyperlink ref="BA20" r:id="rId114" xr:uid="{080618EA-2DEF-479D-82CD-F61076A7E41B}"/>
+    <hyperlink ref="BA21" r:id="rId115" xr:uid="{A9C8C6F0-DE6E-4EB9-871B-F106E0BCFB8B}"/>
+    <hyperlink ref="BA22" r:id="rId116" xr:uid="{FE321390-15EF-451E-9F9E-C80B543C5A11}"/>
+    <hyperlink ref="BA23" r:id="rId117" xr:uid="{313B98A9-6FCE-4DCE-A251-D5F188F6F88E}"/>
+    <hyperlink ref="BA24" r:id="rId118" xr:uid="{150B704A-0B2E-4822-B767-4D27CEBF9DF8}"/>
+    <hyperlink ref="BA25" r:id="rId119" xr:uid="{4CA00F3E-582B-4E64-BE24-599F8270A784}"/>
+    <hyperlink ref="BA26" r:id="rId120" xr:uid="{C9ADAA93-351D-401A-B916-33915CE73013}"/>
+    <hyperlink ref="BA27" r:id="rId121" display="www.inloggen.vgz.nl" xr:uid="{A6F5ECBC-E26E-4A20-9B8B-A9CBA50BF8E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9350,10 +9379,10 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -9361,111 +9390,111 @@
         <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
         <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="D4" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="C5" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="D5" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="C6" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="D6" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="B7" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="C7" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D7" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="C8" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="D8" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="B9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="C9" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="D9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="B10" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="D10" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -9473,24 +9502,24 @@
         <v>179</v>
       </c>
       <c r="B11" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C11" t="s">
         <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -9498,52 +9527,52 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="B13" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="C13" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="D13" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="B14" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C14" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="D14" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="C15" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="B16" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="D16" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -10095,8 +10124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FB691B-88E4-4552-BE42-2A756A8BB771}">
   <dimension ref="A2:F122"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10543,7 +10572,7 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Steps in making parsing results.
</commit_message>
<xml_diff>
--- a/data_health_insurance.xlsx
+++ b/data_health_insurance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marij\PycharmProjects\health_insurance_cloud_networking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8487DFA-E5E4-4960-8941-D573906243F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009C490E-09E7-4390-AB98-9A40CBA2EB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2136,7 +2136,7 @@
   <dimension ref="A1:BV29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG34" sqref="AG34"/>
+      <selection activeCell="AI29" sqref="AI29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finalising, not this code, it is a mess
</commit_message>
<xml_diff>
--- a/data_health_insurance.xlsx
+++ b/data_health_insurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marij\PycharmProjects\health_insurance_cloud_networking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59788CAF-83B1-4CC2-866B-128CDDE1CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0CBA45-C63A-4A32-90BD-21344626C5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30195" yWindow="1395" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="458">
   <si>
     <t>Company</t>
   </si>
@@ -1029,9 +1029,6 @@
   </si>
   <si>
     <t>Amazon germany</t>
-  </si>
-  <si>
-    <t>Amazone</t>
   </si>
   <si>
     <t>Home in Europa</t>
@@ -1489,51 +1486,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="49">
     <dxf>
       <fill>
         <patternFill>
@@ -1602,93 +1555,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1774,121 +1641,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1961,115 +1714,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="7" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -2477,80 +2122,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BX29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BG11" sqref="BG11"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK15" sqref="AK15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="11" width="46.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="8" max="11" width="46.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
-    <col min="16" max="16" width="16.109375" customWidth="1"/>
-    <col min="17" max="17" width="21.88671875" customWidth="1"/>
-    <col min="18" max="18" width="9.88671875" customWidth="1"/>
-    <col min="19" max="19" width="28.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="28.28515625" customWidth="1"/>
     <col min="20" max="20" width="28" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" customWidth="1"/>
-    <col min="22" max="22" width="27.33203125" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="27.28515625" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="17.6640625" customWidth="1"/>
-    <col min="26" max="26" width="13.5546875" customWidth="1"/>
-    <col min="27" max="27" width="12.109375" customWidth="1"/>
-    <col min="28" max="28" width="19.6640625" customWidth="1"/>
-    <col min="29" max="31" width="16.44140625" customWidth="1"/>
-    <col min="32" max="33" width="68.109375" customWidth="1"/>
-    <col min="34" max="34" width="25.33203125" customWidth="1"/>
-    <col min="35" max="38" width="21.5546875" customWidth="1"/>
-    <col min="39" max="39" width="46.44140625" customWidth="1"/>
-    <col min="40" max="40" width="15.44140625" customWidth="1"/>
-    <col min="41" max="41" width="21.109375" customWidth="1"/>
-    <col min="42" max="42" width="24.6640625" customWidth="1"/>
-    <col min="43" max="43" width="14.88671875" customWidth="1"/>
-    <col min="44" max="44" width="32.88671875" customWidth="1"/>
-    <col min="45" max="45" width="32.109375" customWidth="1"/>
-    <col min="46" max="46" width="24.5546875" customWidth="1"/>
-    <col min="47" max="47" width="32.109375" customWidth="1"/>
-    <col min="48" max="48" width="15.44140625" customWidth="1"/>
-    <col min="49" max="49" width="20.44140625" customWidth="1"/>
-    <col min="50" max="50" width="21.33203125" customWidth="1"/>
-    <col min="51" max="51" width="17.6640625" customWidth="1"/>
-    <col min="52" max="52" width="18.33203125" customWidth="1"/>
-    <col min="53" max="53" width="24.33203125" customWidth="1"/>
-    <col min="54" max="55" width="20.6640625" customWidth="1"/>
-    <col min="56" max="56" width="37.6640625" customWidth="1"/>
-    <col min="57" max="57" width="25.6640625" customWidth="1"/>
-    <col min="58" max="59" width="20.109375" customWidth="1"/>
-    <col min="60" max="61" width="29.33203125" customWidth="1"/>
-    <col min="62" max="62" width="10.88671875" customWidth="1"/>
-    <col min="63" max="63" width="16.6640625" customWidth="1"/>
-    <col min="64" max="64" width="21.33203125" customWidth="1"/>
-    <col min="65" max="65" width="11.33203125" customWidth="1"/>
-    <col min="66" max="66" width="28.33203125" customWidth="1"/>
-    <col min="67" max="67" width="48.88671875" customWidth="1"/>
-    <col min="68" max="68" width="19.109375" customWidth="1"/>
+    <col min="25" max="25" width="17.7109375" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" customWidth="1"/>
+    <col min="28" max="28" width="19.7109375" customWidth="1"/>
+    <col min="29" max="31" width="16.42578125" customWidth="1"/>
+    <col min="32" max="33" width="68.140625" customWidth="1"/>
+    <col min="34" max="34" width="25.28515625" customWidth="1"/>
+    <col min="35" max="38" width="21.5703125" customWidth="1"/>
+    <col min="39" max="39" width="46.42578125" customWidth="1"/>
+    <col min="40" max="40" width="15.42578125" customWidth="1"/>
+    <col min="41" max="41" width="21.140625" customWidth="1"/>
+    <col min="42" max="42" width="24.7109375" customWidth="1"/>
+    <col min="43" max="43" width="14.85546875" customWidth="1"/>
+    <col min="44" max="44" width="32.85546875" customWidth="1"/>
+    <col min="45" max="45" width="32.140625" customWidth="1"/>
+    <col min="46" max="46" width="24.5703125" customWidth="1"/>
+    <col min="47" max="47" width="32.140625" customWidth="1"/>
+    <col min="48" max="48" width="15.42578125" customWidth="1"/>
+    <col min="49" max="49" width="20.42578125" customWidth="1"/>
+    <col min="50" max="50" width="21.28515625" customWidth="1"/>
+    <col min="51" max="51" width="17.7109375" customWidth="1"/>
+    <col min="52" max="52" width="18.28515625" customWidth="1"/>
+    <col min="53" max="53" width="24.28515625" customWidth="1"/>
+    <col min="54" max="55" width="20.7109375" customWidth="1"/>
+    <col min="56" max="56" width="37.7109375" customWidth="1"/>
+    <col min="57" max="57" width="25.7109375" customWidth="1"/>
+    <col min="58" max="59" width="20.140625" customWidth="1"/>
+    <col min="60" max="61" width="29.28515625" customWidth="1"/>
+    <col min="62" max="62" width="10.85546875" customWidth="1"/>
+    <col min="63" max="63" width="16.7109375" customWidth="1"/>
+    <col min="64" max="64" width="21.28515625" customWidth="1"/>
+    <col min="65" max="65" width="11.28515625" customWidth="1"/>
+    <col min="66" max="66" width="28.28515625" customWidth="1"/>
+    <col min="67" max="67" width="48.85546875" customWidth="1"/>
+    <col min="68" max="68" width="19.140625" customWidth="1"/>
     <col min="69" max="69" width="27" customWidth="1"/>
-    <col min="70" max="70" width="9.33203125" customWidth="1"/>
-    <col min="71" max="71" width="14.88671875" customWidth="1"/>
-    <col min="72" max="72" width="15.44140625" customWidth="1"/>
-    <col min="73" max="73" width="12.109375" customWidth="1"/>
-    <col min="74" max="74" width="12.44140625" customWidth="1"/>
+    <col min="70" max="70" width="9.28515625" customWidth="1"/>
+    <col min="71" max="71" width="14.85546875" customWidth="1"/>
+    <col min="72" max="72" width="15.42578125" customWidth="1"/>
+    <col min="73" max="73" width="12.140625" customWidth="1"/>
+    <col min="74" max="74" width="12.42578125" customWidth="1"/>
     <col min="75" max="75" width="18" customWidth="1"/>
-    <col min="76" max="76" width="15.33203125" customWidth="1"/>
+    <col min="76" max="76" width="15.28515625" customWidth="1"/>
     <col min="77" max="81" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2576,7 +2221,7 @@
         <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J1" t="s">
         <v>261</v>
@@ -2585,7 +2230,7 @@
         <v>169</v>
       </c>
       <c r="L1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M1" t="s">
         <v>325</v>
@@ -2627,7 +2272,7 @@
         <v>160</v>
       </c>
       <c r="Z1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AA1" t="s">
         <v>135</v>
@@ -2639,31 +2284,31 @@
         <v>137</v>
       </c>
       <c r="AD1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AE1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AF1" t="s">
         <v>133</v>
       </c>
       <c r="AG1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AH1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AI1" t="s">
         <v>161</v>
       </c>
       <c r="AJ1" t="s">
+        <v>456</v>
+      </c>
+      <c r="AK1" t="s">
         <v>457</v>
       </c>
-      <c r="AK1" t="s">
-        <v>458</v>
-      </c>
       <c r="AL1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AM1" t="s">
         <v>185</v>
@@ -2702,7 +2347,7 @@
         <v>168</v>
       </c>
       <c r="AY1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AZ1" t="s">
         <v>139</v>
@@ -2714,10 +2359,10 @@
         <v>141</v>
       </c>
       <c r="BC1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="BD1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="BE1" t="s">
         <v>265</v>
@@ -2726,7 +2371,7 @@
         <v>266</v>
       </c>
       <c r="BG1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="BH1" t="s">
         <v>142</v>
@@ -2780,7 +2425,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2806,7 +2451,7 @@
         <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J2" t="s">
         <v>241</v>
@@ -2818,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N2" t="s">
         <v>300</v>
@@ -2875,10 +2520,10 @@
         <v>1</v>
       </c>
       <c r="AF2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AG2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AH2" t="s">
         <v>241</v>
@@ -2893,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM2" t="s">
         <v>300</v>
@@ -2947,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="BE2" t="s">
         <v>268</v>
@@ -3010,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3036,7 +2681,7 @@
         <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J3" t="s">
         <v>241</v>
@@ -3048,7 +2693,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N3" t="s">
         <v>300</v>
@@ -3105,10 +2750,10 @@
         <v>1</v>
       </c>
       <c r="AF3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AG3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AH3" t="s">
         <v>241</v>
@@ -3123,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM3" t="s">
         <v>300</v>
@@ -3177,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="BD3" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BE3" t="s">
         <v>268</v>
@@ -3240,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3266,7 +2911,7 @@
         <v>73</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J4" t="s">
         <v>241</v>
@@ -3278,7 +2923,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N4" t="s">
         <v>300</v>
@@ -3335,16 +2980,16 @@
         <v>0</v>
       </c>
       <c r="AF4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AG4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AH4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AI4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -3404,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="BD4" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BE4" t="s">
         <v>268</v>
@@ -3467,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3493,7 +3138,7 @@
         <v>77</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J5" t="s">
         <v>241</v>
@@ -3505,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N5" t="s">
         <v>300</v>
@@ -3562,10 +3207,10 @@
         <v>1</v>
       </c>
       <c r="AF5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AG5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AH5" t="s">
         <v>241</v>
@@ -3580,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM5" t="s">
         <v>300</v>
@@ -3634,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="BD5" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BE5" t="s">
         <v>268</v>
@@ -3697,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3723,7 +3368,7 @@
         <v>78</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J6" t="s">
         <v>241</v>
@@ -3735,7 +3380,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N6" t="s">
         <v>300</v>
@@ -3792,10 +3437,10 @@
         <v>1</v>
       </c>
       <c r="AF6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AG6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AH6" t="s">
         <v>241</v>
@@ -3810,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM6" t="s">
         <v>300</v>
@@ -3864,7 +3509,7 @@
         <v>0</v>
       </c>
       <c r="BD6" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="BE6" t="s">
         <v>268</v>
@@ -3927,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3953,7 +3598,7 @@
         <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J7" t="s">
         <v>243</v>
@@ -3962,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N7" t="s">
         <v>9</v>
@@ -4019,10 +3664,10 @@
         <v>1</v>
       </c>
       <c r="AF7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AH7" t="s">
         <v>243</v>
@@ -4031,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="AL7" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM7" t="s">
         <v>9</v>
@@ -4085,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="BD7" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="BE7" t="s">
         <v>272</v>
@@ -4148,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -4174,7 +3819,7 @@
         <v>84</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J8" t="s">
         <v>243</v>
@@ -4183,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N8" t="s">
         <v>9</v>
@@ -4240,10 +3885,10 @@
         <v>1</v>
       </c>
       <c r="AF8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AG8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AH8" t="s">
         <v>243</v>
@@ -4252,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM8" t="s">
         <v>9</v>
@@ -4306,7 +3951,7 @@
         <v>0</v>
       </c>
       <c r="BD8" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="BE8" t="s">
         <v>272</v>
@@ -4369,7 +4014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4395,7 +4040,7 @@
         <v>85</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J9" t="s">
         <v>244</v>
@@ -4404,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N9" t="s">
         <v>322</v>
@@ -4461,10 +4106,10 @@
         <v>1</v>
       </c>
       <c r="AF9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AG9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AH9" t="s">
         <v>244</v>
@@ -4473,7 +4118,7 @@
         <v>0</v>
       </c>
       <c r="AL9" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AM9" t="s">
         <v>322</v>
@@ -4527,7 +4172,7 @@
         <v>0</v>
       </c>
       <c r="BD9" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="BE9" s="3" t="s">
         <v>273</v>
@@ -4590,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -4616,7 +4261,7 @@
         <v>246</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>245</v>
@@ -4625,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N10" t="s">
         <v>322</v>
@@ -4682,10 +4327,10 @@
         <v>1</v>
       </c>
       <c r="AF10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AG10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AH10" s="1" t="s">
         <v>245</v>
@@ -4694,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="AL10" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM10" t="s">
         <v>322</v>
@@ -4748,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="BD10" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="BE10" s="3" t="s">
         <v>273</v>
@@ -4811,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -4837,7 +4482,7 @@
         <v>64</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>244</v>
@@ -4846,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N11" t="s">
         <v>322</v>
@@ -4903,10 +4548,10 @@
         <v>1</v>
       </c>
       <c r="AF11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AG11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AH11" s="1" t="s">
         <v>244</v>
@@ -4915,7 +4560,7 @@
         <v>0</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AM11" t="s">
         <v>322</v>
@@ -4969,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="BD11" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BE11" s="3" t="s">
         <v>273</v>
@@ -5032,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5058,7 +4703,7 @@
         <v>89</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>252</v>
@@ -5127,10 +4772,10 @@
         <v>1</v>
       </c>
       <c r="AF12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AG12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AH12" s="1" t="s">
         <v>252</v>
@@ -5196,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="BD12" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="BE12" s="3" t="s">
         <v>273</v>
@@ -5259,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -5285,7 +4930,7 @@
         <v>74</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>249</v>
@@ -5354,10 +4999,10 @@
         <v>1</v>
       </c>
       <c r="AF13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AG13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AH13" s="1" t="s">
         <v>249</v>
@@ -5423,7 +5068,7 @@
         <v>0</v>
       </c>
       <c r="BD13" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="BE13" s="3" t="s">
         <v>273</v>
@@ -5486,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -5512,7 +5157,7 @@
         <v>65</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>251</v>
@@ -5524,7 +5169,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N14" t="s">
         <v>322</v>
@@ -5581,10 +5226,10 @@
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AG14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AH14" s="1" t="s">
         <v>251</v>
@@ -5596,7 +5241,7 @@
         <v>0</v>
       </c>
       <c r="AL14" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM14" t="s">
         <v>322</v>
@@ -5650,7 +5295,7 @@
         <v>0</v>
       </c>
       <c r="BD14" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BE14" t="s">
         <v>251</v>
@@ -5713,7 +5358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -5739,7 +5384,7 @@
         <v>91</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>251</v>
@@ -5751,7 +5396,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N15" t="s">
         <v>322</v>
@@ -5808,10 +5453,10 @@
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AG15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AH15" s="1" t="s">
         <v>251</v>
@@ -5823,7 +5468,7 @@
         <v>0</v>
       </c>
       <c r="AL15" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM15" t="s">
         <v>322</v>
@@ -5877,7 +5522,7 @@
         <v>0</v>
       </c>
       <c r="BD15" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="BE15" t="s">
         <v>251</v>
@@ -5940,7 +5585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -5966,7 +5611,7 @@
         <v>90</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>253</v>
@@ -5975,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N16" t="s">
         <v>300</v>
@@ -6032,22 +5677,22 @@
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AG16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AH16" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AI16" t="s">
         <v>387</v>
       </c>
-      <c r="AI16" t="s">
-        <v>388</v>
-      </c>
       <c r="AJ16">
         <v>1</v>
       </c>
       <c r="AK16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AL16" s="1" t="s">
         <v>323</v>
@@ -6104,13 +5749,13 @@
         <v>0</v>
       </c>
       <c r="BD16" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="BE16" t="s">
+        <v>386</v>
+      </c>
+      <c r="BF16" t="s">
         <v>387</v>
-      </c>
-      <c r="BF16" t="s">
-        <v>388</v>
       </c>
       <c r="BG16" s="3">
         <v>1</v>
@@ -6167,7 +5812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -6193,7 +5838,7 @@
         <v>92</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>255</v>
@@ -6262,22 +5907,22 @@
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AG17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AH17" t="s">
+        <v>384</v>
+      </c>
+      <c r="AI17" t="s">
         <v>385</v>
       </c>
-      <c r="AI17" t="s">
-        <v>386</v>
-      </c>
       <c r="AJ17">
         <v>1</v>
       </c>
       <c r="AK17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AL17" s="1" t="s">
         <v>306</v>
@@ -6334,7 +5979,7 @@
         <v>0</v>
       </c>
       <c r="BD17" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="BE17" t="s">
         <v>282</v>
@@ -6394,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -6420,7 +6065,7 @@
         <v>93</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>258</v>
@@ -6429,7 +6074,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N18" t="s">
         <v>300</v>
@@ -6486,10 +6131,10 @@
         <v>1</v>
       </c>
       <c r="AF18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AG18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AH18" s="1" t="s">
         <v>258</v>
@@ -6498,7 +6143,7 @@
         <v>0</v>
       </c>
       <c r="AL18" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM18" t="s">
         <v>300</v>
@@ -6552,7 +6197,7 @@
         <v>0</v>
       </c>
       <c r="BD18" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="BE18" t="s">
         <v>273</v>
@@ -6615,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -6641,7 +6286,7 @@
         <v>66</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>258</v>
@@ -6650,7 +6295,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N19" t="s">
         <v>300</v>
@@ -6707,10 +6352,10 @@
         <v>1</v>
       </c>
       <c r="AF19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AG19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AH19" s="1" t="s">
         <v>258</v>
@@ -6719,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="AL19" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM19" t="s">
         <v>300</v>
@@ -6773,7 +6418,7 @@
         <v>0</v>
       </c>
       <c r="BD19" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="BE19" t="s">
         <v>273</v>
@@ -6836,7 +6481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -6862,7 +6507,7 @@
         <v>67</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>258</v>
@@ -6871,7 +6516,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N20" t="s">
         <v>300</v>
@@ -6928,10 +6573,10 @@
         <v>1</v>
       </c>
       <c r="AF20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AG20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AH20" s="1" t="s">
         <v>258</v>
@@ -6940,7 +6585,7 @@
         <v>0</v>
       </c>
       <c r="AL20" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM20" t="s">
         <v>300</v>
@@ -6994,7 +6639,7 @@
         <v>0</v>
       </c>
       <c r="BD20" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="BE20" t="s">
         <v>273</v>
@@ -7057,7 +6702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -7083,7 +6728,7 @@
         <v>94</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>259</v>
@@ -7152,16 +6797,16 @@
         <v>0</v>
       </c>
       <c r="AF21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AG21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AH21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AI21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AJ21">
         <v>0</v>
@@ -7170,10 +6815,10 @@
         <v>326</v>
       </c>
       <c r="AM21" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="AN21" s="1" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="AO21">
         <v>1</v>
@@ -7221,7 +6866,7 @@
         <v>0</v>
       </c>
       <c r="BD21" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="BE21" t="s">
         <v>268</v>
@@ -7284,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -7310,7 +6955,7 @@
         <v>83</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>255</v>
@@ -7379,16 +7024,16 @@
         <v>0</v>
       </c>
       <c r="AF22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AG22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AH22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AI22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AJ22">
         <v>0</v>
@@ -7397,10 +7042,10 @@
         <v>326</v>
       </c>
       <c r="AM22" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="AO22">
         <v>1</v>
@@ -7448,7 +7093,7 @@
         <v>0</v>
       </c>
       <c r="BD22" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BE22" t="s">
         <v>281</v>
@@ -7511,7 +7156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -7537,7 +7182,7 @@
         <v>88</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>262</v>
@@ -7546,7 +7191,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N23" t="s">
         <v>300</v>
@@ -7603,10 +7248,10 @@
         <v>1</v>
       </c>
       <c r="AF23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AG23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AH23" s="1" t="s">
         <v>262</v>
@@ -7622,7 +7267,7 @@
         <v>0</v>
       </c>
       <c r="AL23" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM23" t="s">
         <v>300</v>
@@ -7676,7 +7321,7 @@
         <v>0</v>
       </c>
       <c r="BD23" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="BE23" t="s">
         <v>283</v>
@@ -7736,7 +7381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -7762,7 +7407,7 @@
         <v>82</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>263</v>
@@ -7771,7 +7416,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N24" t="s">
         <v>300</v>
@@ -7828,10 +7473,10 @@
         <v>1</v>
       </c>
       <c r="AF24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AG24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AH24" s="1" t="s">
         <v>263</v>
@@ -7843,7 +7488,7 @@
         <v>0</v>
       </c>
       <c r="AL24" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM24" t="s">
         <v>300</v>
@@ -7957,7 +7602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -7983,7 +7628,7 @@
         <v>68</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>263</v>
@@ -7992,7 +7637,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N25" t="s">
         <v>300</v>
@@ -8049,10 +7694,10 @@
         <v>1</v>
       </c>
       <c r="AF25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AG25" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AH25" s="1" t="s">
         <v>263</v>
@@ -8064,7 +7709,7 @@
         <v>0</v>
       </c>
       <c r="AL25" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM25" t="s">
         <v>300</v>
@@ -8118,7 +7763,7 @@
         <v>0</v>
       </c>
       <c r="BD25" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BE25" t="s">
         <v>287</v>
@@ -8178,7 +7823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -8204,7 +7849,7 @@
         <v>75</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J26" t="s">
         <v>240</v>
@@ -8213,13 +7858,13 @@
         <v>0</v>
       </c>
       <c r="M26" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="N26" t="s">
         <v>345</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -8270,10 +7915,10 @@
         <v>1</v>
       </c>
       <c r="AF26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AG26" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AH26" t="s">
         <v>240</v>
@@ -8282,13 +7927,13 @@
         <v>0</v>
       </c>
       <c r="AL26" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="AM26" t="s">
         <v>345</v>
       </c>
-      <c r="AM26" t="s">
+      <c r="AN26" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="AN26" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="AO26">
         <v>1</v>
@@ -8336,7 +7981,7 @@
         <v>0</v>
       </c>
       <c r="BD26" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="BE26" t="s">
         <v>288</v>
@@ -8396,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -8422,7 +8067,7 @@
         <v>80</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J27" t="s">
         <v>239</v>
@@ -8431,13 +8076,13 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P27">
         <v>1</v>
@@ -8488,10 +8133,10 @@
         <v>1</v>
       </c>
       <c r="AF27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AG27" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AH27" t="s">
         <v>239</v>
@@ -8500,13 +8145,13 @@
         <v>0</v>
       </c>
       <c r="AL27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AN27" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AO27">
         <v>1</v>
@@ -8614,7 +8259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -8637,10 +8282,10 @@
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J28" t="s">
         <v>175</v>
@@ -8652,10 +8297,10 @@
         <v>177</v>
       </c>
       <c r="N28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -8706,10 +8351,10 @@
         <v>1</v>
       </c>
       <c r="AF28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AG28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AH28" t="s">
         <v>175</v>
@@ -8722,10 +8367,10 @@
         <v>177</v>
       </c>
       <c r="AM28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AN28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AO28">
         <v>1</v>
@@ -8833,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:76" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -8859,7 +8504,7 @@
         <v>81</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>256</v>
@@ -8928,13 +8573,13 @@
         <v>0</v>
       </c>
       <c r="AF29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AG29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AH29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AJ29">
         <v>0</v>
@@ -9191,8 +8836,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="116">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="duplicateValues" dxfId="43" priority="115"/>
-    <cfRule type="colorScale" priority="116">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L29">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -9297,16 +8952,16 @@
     <cfRule type="duplicateValues" dxfId="32" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI2:AI3">
-    <cfRule type="duplicateValues" dxfId="31" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="70"/>
     <cfRule type="top10" priority="71" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5:AI6">
     <cfRule type="duplicateValues" dxfId="28" priority="61"/>
-    <cfRule type="top10" priority="62" percent="1" rank="10"/>
     <cfRule type="duplicateValues" dxfId="27" priority="63"/>
     <cfRule type="duplicateValues" dxfId="26" priority="64"/>
+    <cfRule type="top10" priority="62" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI7:AI8">
     <cfRule type="duplicateValues" dxfId="25" priority="52"/>
@@ -9317,14 +8972,10 @@
   <conditionalFormatting sqref="AI9:AI13">
     <cfRule type="duplicateValues" dxfId="22" priority="43"/>
     <cfRule type="top10" priority="44" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="45"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI14">
-    <cfRule type="duplicateValues" dxfId="19" priority="18"/>
-    <cfRule type="top10" priority="19" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="21"/>
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -9333,6 +8984,10 @@
         <color theme="9" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
+    <cfRule type="top10" priority="19" percent="1" rank="10"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI15">
     <cfRule type="duplicateValues" dxfId="16" priority="12"/>
@@ -9355,10 +9010,10 @@
     <cfRule type="duplicateValues" dxfId="11" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI23:AI25">
-    <cfRule type="duplicateValues" dxfId="10" priority="25"/>
     <cfRule type="top10" priority="26" percent="1" rank="10"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI26">
     <cfRule type="duplicateValues" dxfId="7" priority="79"/>
@@ -9840,9 +9495,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BE2:BE29">
-    <cfRule type="duplicateValues" dxfId="1" priority="122"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BD28:BE28 BE17:BJ17 F2:F29 BD29:BJ29 BD22:BG27 BJ22:BJ27 BD12:BJ13 BD14:BG16 BD21:BJ21 BD18:BG20 BI18:BJ20 BI14:BJ16 BD9:BJ10 BD7:BG8 BI7:BJ8 BD3:BD6 BE2:BJ6 BG11 BG28:BJ28">
     <cfRule type="colorScale" priority="135">
       <colorScale>
@@ -9852,6 +9504,9 @@
         <color theme="9" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BE2:BE29">
+    <cfRule type="duplicateValues" dxfId="1" priority="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM2:BQ29">
     <cfRule type="colorScale" priority="137">
@@ -9877,16 +9532,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="BS2:BS29">
     <cfRule type="colorScale" priority="138">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5" tint="0.79998168889431442"/>
-        <color theme="9" tint="0.79998168889431442"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L29">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10030,9 +9675,9 @@
       <selection activeCell="A18" sqref="A18:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>301</v>
       </c>
@@ -10040,7 +9685,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -10054,7 +9699,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -10068,7 +9713,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>297</v>
       </c>
@@ -10082,7 +9727,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>304</v>
       </c>
@@ -10096,7 +9741,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>310</v>
       </c>
@@ -10110,7 +9755,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>315</v>
       </c>
@@ -10124,7 +9769,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>320</v>
       </c>
@@ -10138,7 +9783,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>328</v>
       </c>
@@ -10152,85 +9797,85 @@
         <v>329</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
         <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" t="s">
+        <v>336</v>
+      </c>
+      <c r="D13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B14" t="s">
+        <v>340</v>
+      </c>
+      <c r="C14" t="s">
         <v>339</v>
       </c>
-      <c r="B13" t="s">
-        <v>338</v>
-      </c>
-      <c r="C13" t="s">
-        <v>337</v>
-      </c>
-      <c r="D13" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>343</v>
+      </c>
+      <c r="C15" t="s">
         <v>342</v>
       </c>
-      <c r="B14" t="s">
-        <v>341</v>
-      </c>
-      <c r="C14" t="s">
-        <v>340</v>
-      </c>
-      <c r="D14" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>344</v>
-      </c>
-      <c r="C15" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B16" t="s">
+        <v>347</v>
+      </c>
+      <c r="C16" t="s">
         <v>348</v>
       </c>
-      <c r="C16" t="s">
-        <v>349</v>
-      </c>
       <c r="D16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>144</v>
       </c>
@@ -10238,7 +9883,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>146</v>
       </c>
@@ -10277,15 +9922,15 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10299,7 +9944,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -10313,7 +9958,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -10324,7 +9969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -10335,7 +9980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
@@ -10346,7 +9991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -10357,7 +10002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -10371,7 +10016,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -10382,7 +10027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -10393,7 +10038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -10404,7 +10049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -10415,7 +10060,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -10426,7 +10071,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -10437,7 +10082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -10448,7 +10093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -10459,7 +10104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10470,7 +10115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -10481,7 +10126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -10492,7 +10137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -10503,7 +10148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
@@ -10514,7 +10159,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -10525,7 +10170,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -10536,7 +10181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -10547,7 +10192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -10558,7 +10203,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -10569,7 +10214,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -10580,7 +10225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -10591,7 +10236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -10602,7 +10247,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -10613,7 +10258,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -10624,7 +10269,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -10635,7 +10280,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -10646,7 +10291,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -10657,7 +10302,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -10668,7 +10313,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -10679,7 +10324,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -10690,7 +10335,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -10701,7 +10346,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -10712,7 +10357,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -10723,7 +10368,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -10734,7 +10379,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -10745,7 +10390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
@@ -10756,7 +10401,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -10783,52 +10428,52 @@
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="23.109375" customWidth="1"/>
+    <col min="1" max="7" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -10836,7 +10481,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -10844,7 +10489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -10852,7 +10497,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -10860,7 +10505,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -10871,7 +10516,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -10879,7 +10524,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -10887,7 +10532,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -10895,7 +10540,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -10903,7 +10548,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -10914,7 +10559,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -10922,7 +10567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -10930,7 +10575,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -10938,7 +10583,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -10946,7 +10591,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -10954,7 +10599,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -10962,12 +10607,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -10975,97 +10620,97 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>211</v>
       </c>
@@ -11073,7 +10718,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>231</v>
       </c>
@@ -11084,7 +10729,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>213</v>
       </c>
@@ -11092,17 +10737,17 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>218</v>
       </c>
@@ -11116,27 +10761,27 @@
         <v>234</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>225</v>
       </c>
@@ -11153,7 +10798,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
         <v>236</v>
       </c>
@@ -11161,12 +10806,12 @@
         <v>237</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>203</v>
       </c>
@@ -11174,12 +10819,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>206</v>
       </c>
@@ -11187,12 +10832,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>209</v>
       </c>
@@ -11200,32 +10845,32 @@
         <v>210</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>270</v>
       </c>

</xml_diff>